<commit_message>
fangesegments: updated unit test for PolynomialLFlangeSegment
</commit_message>
<xml_diff>
--- a/validations/flangesegments.PolynomialLFlangeSegment/BnB_ReferenceFlange-Results-ShapeFactor-1.2.xlsx
+++ b/validations/flangesegments.PolynomialLFlangeSegment/BnB_ReferenceFlange-Results-ShapeFactor-1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelloB\mdb\!Progetti\!KCI\!SP2200052 - Bolt &amp; Beautiful\!pyflange-package\validations\flangesegments.PolynomialLFlangeSegment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C505DF24-2698-4387-964F-C3B50CFC2909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D73949C-CD35-4919-A71D-BDE921882F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
+    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Gap30deg" sheetId="2" r:id="rId1"/>
@@ -5053,7 +5053,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="179">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5495,31 +5495,10 @@
     <xf numFmtId="0" fontId="65" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="170" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5531,43 +5510,35 @@
     <xf numFmtId="0" fontId="25" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="12" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="18" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -19759,7 +19730,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="45720" tIns="36576" rIns="45720" bIns="36576" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -20127,8 +20098,8 @@
   <dimension ref="A1:DJ180"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J152" sqref="J152"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N85" sqref="N85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -20173,32 +20144,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
+      <c r="B3" s="162"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="162"/>
+      <c r="F3" s="162"/>
+      <c r="G3" s="162"/>
+      <c r="H3" s="162"/>
+      <c r="I3" s="162"/>
+      <c r="J3" s="162"/>
+      <c r="K3" s="162"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="161" t="s">
+      <c r="B4" s="163" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -20214,12 +20185,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
+      <c r="B5" s="155"/>
+      <c r="C5" s="156"/>
+      <c r="D5" s="156"/>
+      <c r="E5" s="156"/>
+      <c r="F5" s="156"/>
+      <c r="G5" s="157"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -20227,12 +20198,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="B6" s="155"/>
+      <c r="C6" s="156"/>
+      <c r="D6" s="156"/>
+      <c r="E6" s="156"/>
+      <c r="F6" s="156"/>
+      <c r="G6" s="157"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -20240,12 +20211,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="162"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="B7" s="155"/>
+      <c r="C7" s="156"/>
+      <c r="D7" s="156"/>
+      <c r="E7" s="156"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="157"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -20253,12 +20224,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="164"/>
+      <c r="B8" s="155"/>
+      <c r="C8" s="156"/>
+      <c r="D8" s="156"/>
+      <c r="E8" s="156"/>
+      <c r="F8" s="156"/>
+      <c r="G8" s="157"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -20266,12 +20237,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
+      <c r="B9" s="155"/>
+      <c r="C9" s="156"/>
+      <c r="D9" s="156"/>
+      <c r="E9" s="156"/>
+      <c r="F9" s="156"/>
+      <c r="G9" s="157"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -20319,112 +20290,112 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="155" t="s">
+      <c r="B13" s="158" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="155"/>
-      <c r="D13" s="154" t="s">
+      <c r="C13" s="158"/>
+      <c r="D13" s="160" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="154"/>
-      <c r="F13" s="154"/>
-      <c r="G13" s="154"/>
-      <c r="H13" s="154"/>
-      <c r="I13" s="154"/>
-      <c r="J13" s="154"/>
-      <c r="K13" s="154"/>
+      <c r="E13" s="160"/>
+      <c r="F13" s="160"/>
+      <c r="G13" s="160"/>
+      <c r="H13" s="160"/>
+      <c r="I13" s="160"/>
+      <c r="J13" s="160"/>
+      <c r="K13" s="160"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="155" t="s">
+      <c r="B14" s="158" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="155"/>
-      <c r="D14" s="154" t="s">
+      <c r="C14" s="158"/>
+      <c r="D14" s="160" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="154"/>
-      <c r="F14" s="154"/>
-      <c r="G14" s="154"/>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="154"/>
-      <c r="K14" s="154"/>
+      <c r="E14" s="160"/>
+      <c r="F14" s="160"/>
+      <c r="G14" s="160"/>
+      <c r="H14" s="160"/>
+      <c r="I14" s="160"/>
+      <c r="J14" s="160"/>
+      <c r="K14" s="160"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="155" t="s">
+      <c r="B15" s="158" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="155"/>
-      <c r="D15" s="154" t="s">
+      <c r="C15" s="158"/>
+      <c r="D15" s="160" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="154"/>
-      <c r="F15" s="154"/>
-      <c r="G15" s="154"/>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="154"/>
-      <c r="K15" s="154"/>
+      <c r="E15" s="160"/>
+      <c r="F15" s="160"/>
+      <c r="G15" s="160"/>
+      <c r="H15" s="160"/>
+      <c r="I15" s="160"/>
+      <c r="J15" s="160"/>
+      <c r="K15" s="160"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="155" t="s">
+      <c r="B16" s="158" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="155"/>
-      <c r="D16" s="154" t="str">
+      <c r="C16" s="158"/>
+      <c r="D16" s="160" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 30° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
+      <c r="E16" s="160"/>
+      <c r="F16" s="160"/>
+      <c r="G16" s="160"/>
+      <c r="H16" s="160"/>
+      <c r="I16" s="160"/>
+      <c r="J16" s="160"/>
+      <c r="K16" s="160"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="155" t="s">
+      <c r="B17" s="158" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="155"/>
-      <c r="D17" s="153">
+      <c r="C17" s="158"/>
+      <c r="D17" s="164">
         <v>0.1</v>
       </c>
-      <c r="E17" s="154"/>
-      <c r="F17" s="154"/>
-      <c r="G17" s="154"/>
-      <c r="H17" s="154"/>
-      <c r="I17" s="154"/>
-      <c r="J17" s="154"/>
-      <c r="K17" s="154"/>
+      <c r="E17" s="160"/>
+      <c r="F17" s="160"/>
+      <c r="G17" s="160"/>
+      <c r="H17" s="160"/>
+      <c r="I17" s="160"/>
+      <c r="J17" s="160"/>
+      <c r="K17" s="160"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="155" t="s">
+      <c r="B18" s="158" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="155"/>
-      <c r="D18" s="165">
+      <c r="C18" s="158"/>
+      <c r="D18" s="159">
         <v>45432</v>
       </c>
-      <c r="E18" s="165"/>
-      <c r="F18" s="165"/>
-      <c r="G18" s="165"/>
-      <c r="H18" s="165"/>
-      <c r="I18" s="165"/>
-      <c r="J18" s="165"/>
-      <c r="K18" s="165"/>
+      <c r="E18" s="159"/>
+      <c r="F18" s="159"/>
+      <c r="G18" s="159"/>
+      <c r="H18" s="159"/>
+      <c r="I18" s="159"/>
+      <c r="J18" s="159"/>
+      <c r="K18" s="159"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -20612,16 +20583,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="156"/>
-      <c r="C28" s="157"/>
-      <c r="D28" s="157"/>
-      <c r="E28" s="157"/>
-      <c r="F28" s="157"/>
-      <c r="G28" s="157"/>
-      <c r="H28" s="157"/>
-      <c r="I28" s="157"/>
-      <c r="J28" s="157"/>
-      <c r="K28" s="158"/>
+      <c r="B28" s="165"/>
+      <c r="C28" s="166"/>
+      <c r="D28" s="166"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="166"/>
+      <c r="H28" s="166"/>
+      <c r="I28" s="166"/>
+      <c r="J28" s="166"/>
+      <c r="K28" s="167"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -24584,6 +24555,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B18:C18"/>
@@ -24594,16 +24571,10 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
     <mergeCell ref="D17:K17"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B28:K28"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="27" priority="5" stopIfTrue="1" operator="between">
@@ -24643,7 +24614,7 @@
   <dimension ref="A1:DJ180"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K85" sqref="K85"/>
     </sheetView>
   </sheetViews>
@@ -24689,32 +24660,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
+      <c r="B3" s="162"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="162"/>
+      <c r="F3" s="162"/>
+      <c r="G3" s="162"/>
+      <c r="H3" s="162"/>
+      <c r="I3" s="162"/>
+      <c r="J3" s="162"/>
+      <c r="K3" s="162"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="161" t="s">
+      <c r="B4" s="163" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -24730,12 +24701,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
+      <c r="B5" s="155"/>
+      <c r="C5" s="156"/>
+      <c r="D5" s="156"/>
+      <c r="E5" s="156"/>
+      <c r="F5" s="156"/>
+      <c r="G5" s="157"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -24743,12 +24714,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="B6" s="155"/>
+      <c r="C6" s="156"/>
+      <c r="D6" s="156"/>
+      <c r="E6" s="156"/>
+      <c r="F6" s="156"/>
+      <c r="G6" s="157"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -24756,12 +24727,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="162"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="B7" s="155"/>
+      <c r="C7" s="156"/>
+      <c r="D7" s="156"/>
+      <c r="E7" s="156"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="157"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -24769,12 +24740,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="164"/>
+      <c r="B8" s="155"/>
+      <c r="C8" s="156"/>
+      <c r="D8" s="156"/>
+      <c r="E8" s="156"/>
+      <c r="F8" s="156"/>
+      <c r="G8" s="157"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -24782,12 +24753,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
+      <c r="B9" s="155"/>
+      <c r="C9" s="156"/>
+      <c r="D9" s="156"/>
+      <c r="E9" s="156"/>
+      <c r="F9" s="156"/>
+      <c r="G9" s="157"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -24835,117 +24806,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="155" t="s">
+      <c r="B13" s="158" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="155"/>
-      <c r="D13" s="154" t="str">
+      <c r="C13" s="158"/>
+      <c r="D13" s="160" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="154"/>
-      <c r="F13" s="154"/>
-      <c r="G13" s="154"/>
-      <c r="H13" s="154"/>
-      <c r="I13" s="154"/>
-      <c r="J13" s="154"/>
-      <c r="K13" s="154"/>
+      <c r="E13" s="160"/>
+      <c r="F13" s="160"/>
+      <c r="G13" s="160"/>
+      <c r="H13" s="160"/>
+      <c r="I13" s="160"/>
+      <c r="J13" s="160"/>
+      <c r="K13" s="160"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="155" t="s">
+      <c r="B14" s="158" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="155"/>
-      <c r="D14" s="154" t="str">
+      <c r="C14" s="158"/>
+      <c r="D14" s="160" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="154"/>
-      <c r="F14" s="154"/>
-      <c r="G14" s="154"/>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="154"/>
-      <c r="K14" s="154"/>
+      <c r="E14" s="160"/>
+      <c r="F14" s="160"/>
+      <c r="G14" s="160"/>
+      <c r="H14" s="160"/>
+      <c r="I14" s="160"/>
+      <c r="J14" s="160"/>
+      <c r="K14" s="160"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="155" t="s">
+      <c r="B15" s="158" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="155"/>
-      <c r="D15" s="154" t="str">
+      <c r="C15" s="158"/>
+      <c r="D15" s="160" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="154"/>
-      <c r="F15" s="154"/>
-      <c r="G15" s="154"/>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="154"/>
-      <c r="K15" s="154"/>
+      <c r="E15" s="160"/>
+      <c r="F15" s="160"/>
+      <c r="G15" s="160"/>
+      <c r="H15" s="160"/>
+      <c r="I15" s="160"/>
+      <c r="J15" s="160"/>
+      <c r="K15" s="160"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="155" t="s">
+      <c r="B16" s="158" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="155"/>
-      <c r="D16" s="154" t="str">
+      <c r="C16" s="158"/>
+      <c r="D16" s="160" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 60° gap size ans shape factor 1.2</v>
       </c>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
+      <c r="E16" s="160"/>
+      <c r="F16" s="160"/>
+      <c r="G16" s="160"/>
+      <c r="H16" s="160"/>
+      <c r="I16" s="160"/>
+      <c r="J16" s="160"/>
+      <c r="K16" s="160"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="155" t="s">
+      <c r="B17" s="158" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="155"/>
-      <c r="D17" s="154">
+      <c r="C17" s="158"/>
+      <c r="D17" s="160">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="154"/>
-      <c r="F17" s="154"/>
-      <c r="G17" s="154"/>
-      <c r="H17" s="154"/>
-      <c r="I17" s="154"/>
-      <c r="J17" s="154"/>
-      <c r="K17" s="154"/>
+      <c r="E17" s="160"/>
+      <c r="F17" s="160"/>
+      <c r="G17" s="160"/>
+      <c r="H17" s="160"/>
+      <c r="I17" s="160"/>
+      <c r="J17" s="160"/>
+      <c r="K17" s="160"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="155" t="s">
+      <c r="B18" s="158" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="155"/>
-      <c r="D18" s="165">
+      <c r="C18" s="158"/>
+      <c r="D18" s="159">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="165"/>
-      <c r="F18" s="165"/>
-      <c r="G18" s="165"/>
-      <c r="H18" s="165"/>
-      <c r="I18" s="165"/>
-      <c r="J18" s="165"/>
-      <c r="K18" s="165"/>
+      <c r="E18" s="159"/>
+      <c r="F18" s="159"/>
+      <c r="G18" s="159"/>
+      <c r="H18" s="159"/>
+      <c r="I18" s="159"/>
+      <c r="J18" s="159"/>
+      <c r="K18" s="159"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -25133,16 +25104,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="156"/>
-      <c r="C28" s="157"/>
-      <c r="D28" s="157"/>
-      <c r="E28" s="157"/>
-      <c r="F28" s="157"/>
-      <c r="G28" s="157"/>
-      <c r="H28" s="157"/>
-      <c r="I28" s="157"/>
-      <c r="J28" s="157"/>
-      <c r="K28" s="158"/>
+      <c r="B28" s="165"/>
+      <c r="C28" s="166"/>
+      <c r="D28" s="166"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="166"/>
+      <c r="H28" s="166"/>
+      <c r="I28" s="166"/>
+      <c r="J28" s="166"/>
+      <c r="K28" s="167"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -29068,6 +29039,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -29081,13 +29059,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="24" priority="3" stopIfTrue="1" operator="between">
@@ -29127,7 +29098,7 @@
   <dimension ref="A1:DJ180"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K86" sqref="K86"/>
     </sheetView>
   </sheetViews>
@@ -29173,32 +29144,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
+      <c r="B3" s="162"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="162"/>
+      <c r="F3" s="162"/>
+      <c r="G3" s="162"/>
+      <c r="H3" s="162"/>
+      <c r="I3" s="162"/>
+      <c r="J3" s="162"/>
+      <c r="K3" s="162"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="161" t="s">
+      <c r="B4" s="163" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -29214,12 +29185,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
+      <c r="B5" s="155"/>
+      <c r="C5" s="156"/>
+      <c r="D5" s="156"/>
+      <c r="E5" s="156"/>
+      <c r="F5" s="156"/>
+      <c r="G5" s="157"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -29227,12 +29198,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="B6" s="155"/>
+      <c r="C6" s="156"/>
+      <c r="D6" s="156"/>
+      <c r="E6" s="156"/>
+      <c r="F6" s="156"/>
+      <c r="G6" s="157"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -29240,12 +29211,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="162"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="B7" s="155"/>
+      <c r="C7" s="156"/>
+      <c r="D7" s="156"/>
+      <c r="E7" s="156"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="157"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -29253,12 +29224,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="164"/>
+      <c r="B8" s="155"/>
+      <c r="C8" s="156"/>
+      <c r="D8" s="156"/>
+      <c r="E8" s="156"/>
+      <c r="F8" s="156"/>
+      <c r="G8" s="157"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -29266,12 +29237,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
+      <c r="B9" s="155"/>
+      <c r="C9" s="156"/>
+      <c r="D9" s="156"/>
+      <c r="E9" s="156"/>
+      <c r="F9" s="156"/>
+      <c r="G9" s="157"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -29319,117 +29290,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="155" t="s">
+      <c r="B13" s="158" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="155"/>
-      <c r="D13" s="154" t="str">
+      <c r="C13" s="158"/>
+      <c r="D13" s="160" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="154"/>
-      <c r="F13" s="154"/>
-      <c r="G13" s="154"/>
-      <c r="H13" s="154"/>
-      <c r="I13" s="154"/>
-      <c r="J13" s="154"/>
-      <c r="K13" s="154"/>
+      <c r="E13" s="160"/>
+      <c r="F13" s="160"/>
+      <c r="G13" s="160"/>
+      <c r="H13" s="160"/>
+      <c r="I13" s="160"/>
+      <c r="J13" s="160"/>
+      <c r="K13" s="160"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="155" t="s">
+      <c r="B14" s="158" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="155"/>
-      <c r="D14" s="154" t="str">
+      <c r="C14" s="158"/>
+      <c r="D14" s="160" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="154"/>
-      <c r="F14" s="154"/>
-      <c r="G14" s="154"/>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="154"/>
-      <c r="K14" s="154"/>
+      <c r="E14" s="160"/>
+      <c r="F14" s="160"/>
+      <c r="G14" s="160"/>
+      <c r="H14" s="160"/>
+      <c r="I14" s="160"/>
+      <c r="J14" s="160"/>
+      <c r="K14" s="160"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="155" t="s">
+      <c r="B15" s="158" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="155"/>
-      <c r="D15" s="154" t="str">
+      <c r="C15" s="158"/>
+      <c r="D15" s="160" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="154"/>
-      <c r="F15" s="154"/>
-      <c r="G15" s="154"/>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="154"/>
-      <c r="K15" s="154"/>
+      <c r="E15" s="160"/>
+      <c r="F15" s="160"/>
+      <c r="G15" s="160"/>
+      <c r="H15" s="160"/>
+      <c r="I15" s="160"/>
+      <c r="J15" s="160"/>
+      <c r="K15" s="160"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="155" t="s">
+      <c r="B16" s="158" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="155"/>
-      <c r="D16" s="154" t="str">
+      <c r="C16" s="158"/>
+      <c r="D16" s="160" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 90° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
+      <c r="E16" s="160"/>
+      <c r="F16" s="160"/>
+      <c r="G16" s="160"/>
+      <c r="H16" s="160"/>
+      <c r="I16" s="160"/>
+      <c r="J16" s="160"/>
+      <c r="K16" s="160"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="155" t="s">
+      <c r="B17" s="158" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="155"/>
-      <c r="D17" s="154">
+      <c r="C17" s="158"/>
+      <c r="D17" s="160">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="154"/>
-      <c r="F17" s="154"/>
-      <c r="G17" s="154"/>
-      <c r="H17" s="154"/>
-      <c r="I17" s="154"/>
-      <c r="J17" s="154"/>
-      <c r="K17" s="154"/>
+      <c r="E17" s="160"/>
+      <c r="F17" s="160"/>
+      <c r="G17" s="160"/>
+      <c r="H17" s="160"/>
+      <c r="I17" s="160"/>
+      <c r="J17" s="160"/>
+      <c r="K17" s="160"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="155" t="s">
+      <c r="B18" s="158" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="155"/>
-      <c r="D18" s="165">
+      <c r="C18" s="158"/>
+      <c r="D18" s="159">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="165"/>
-      <c r="F18" s="165"/>
-      <c r="G18" s="165"/>
-      <c r="H18" s="165"/>
-      <c r="I18" s="165"/>
-      <c r="J18" s="165"/>
-      <c r="K18" s="165"/>
+      <c r="E18" s="159"/>
+      <c r="F18" s="159"/>
+      <c r="G18" s="159"/>
+      <c r="H18" s="159"/>
+      <c r="I18" s="159"/>
+      <c r="J18" s="159"/>
+      <c r="K18" s="159"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -29617,16 +29588,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="156"/>
-      <c r="C28" s="157"/>
-      <c r="D28" s="157"/>
-      <c r="E28" s="157"/>
-      <c r="F28" s="157"/>
-      <c r="G28" s="157"/>
-      <c r="H28" s="157"/>
-      <c r="I28" s="157"/>
-      <c r="J28" s="157"/>
-      <c r="K28" s="158"/>
+      <c r="B28" s="165"/>
+      <c r="C28" s="166"/>
+      <c r="D28" s="166"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="166"/>
+      <c r="H28" s="166"/>
+      <c r="I28" s="166"/>
+      <c r="J28" s="166"/>
+      <c r="K28" s="167"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -33552,6 +33523,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -33565,13 +33543,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="between">
@@ -33610,8 +33581,8 @@
   </sheetPr>
   <dimension ref="A1:DJ180"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O117" sqref="O117"/>
     </sheetView>
   </sheetViews>
@@ -33657,32 +33628,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="161" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
+      <c r="B3" s="162"/>
+      <c r="C3" s="162"/>
+      <c r="D3" s="162"/>
+      <c r="E3" s="162"/>
+      <c r="F3" s="162"/>
+      <c r="G3" s="162"/>
+      <c r="H3" s="162"/>
+      <c r="I3" s="162"/>
+      <c r="J3" s="162"/>
+      <c r="K3" s="162"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="161" t="s">
+      <c r="B4" s="163" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="161"/>
-      <c r="D4" s="161"/>
-      <c r="E4" s="161"/>
-      <c r="F4" s="161"/>
-      <c r="G4" s="161"/>
+      <c r="C4" s="163"/>
+      <c r="D4" s="163"/>
+      <c r="E4" s="163"/>
+      <c r="F4" s="163"/>
+      <c r="G4" s="163"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -33698,12 +33669,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="162"/>
-      <c r="C5" s="163"/>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
-      <c r="F5" s="163"/>
-      <c r="G5" s="164"/>
+      <c r="B5" s="155"/>
+      <c r="C5" s="156"/>
+      <c r="D5" s="156"/>
+      <c r="E5" s="156"/>
+      <c r="F5" s="156"/>
+      <c r="G5" s="157"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -33711,12 +33682,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="162"/>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163"/>
-      <c r="E6" s="163"/>
-      <c r="F6" s="163"/>
-      <c r="G6" s="164"/>
+      <c r="B6" s="155"/>
+      <c r="C6" s="156"/>
+      <c r="D6" s="156"/>
+      <c r="E6" s="156"/>
+      <c r="F6" s="156"/>
+      <c r="G6" s="157"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -33724,12 +33695,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="162"/>
-      <c r="C7" s="163"/>
-      <c r="D7" s="163"/>
-      <c r="E7" s="163"/>
-      <c r="F7" s="163"/>
-      <c r="G7" s="164"/>
+      <c r="B7" s="155"/>
+      <c r="C7" s="156"/>
+      <c r="D7" s="156"/>
+      <c r="E7" s="156"/>
+      <c r="F7" s="156"/>
+      <c r="G7" s="157"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -33737,12 +33708,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="162"/>
-      <c r="C8" s="163"/>
-      <c r="D8" s="163"/>
-      <c r="E8" s="163"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="164"/>
+      <c r="B8" s="155"/>
+      <c r="C8" s="156"/>
+      <c r="D8" s="156"/>
+      <c r="E8" s="156"/>
+      <c r="F8" s="156"/>
+      <c r="G8" s="157"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -33750,12 +33721,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="162"/>
-      <c r="C9" s="163"/>
-      <c r="D9" s="163"/>
-      <c r="E9" s="163"/>
-      <c r="F9" s="163"/>
-      <c r="G9" s="164"/>
+      <c r="B9" s="155"/>
+      <c r="C9" s="156"/>
+      <c r="D9" s="156"/>
+      <c r="E9" s="156"/>
+      <c r="F9" s="156"/>
+      <c r="G9" s="157"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -33803,117 +33774,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="155" t="s">
+      <c r="B13" s="158" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="155"/>
-      <c r="D13" s="154" t="str">
+      <c r="C13" s="158"/>
+      <c r="D13" s="160" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="154"/>
-      <c r="F13" s="154"/>
-      <c r="G13" s="154"/>
-      <c r="H13" s="154"/>
-      <c r="I13" s="154"/>
-      <c r="J13" s="154"/>
-      <c r="K13" s="154"/>
+      <c r="E13" s="160"/>
+      <c r="F13" s="160"/>
+      <c r="G13" s="160"/>
+      <c r="H13" s="160"/>
+      <c r="I13" s="160"/>
+      <c r="J13" s="160"/>
+      <c r="K13" s="160"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="155" t="s">
+      <c r="B14" s="158" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="155"/>
-      <c r="D14" s="154" t="str">
+      <c r="C14" s="158"/>
+      <c r="D14" s="160" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="154"/>
-      <c r="F14" s="154"/>
-      <c r="G14" s="154"/>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
-      <c r="J14" s="154"/>
-      <c r="K14" s="154"/>
+      <c r="E14" s="160"/>
+      <c r="F14" s="160"/>
+      <c r="G14" s="160"/>
+      <c r="H14" s="160"/>
+      <c r="I14" s="160"/>
+      <c r="J14" s="160"/>
+      <c r="K14" s="160"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="155" t="s">
+      <c r="B15" s="158" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="155"/>
-      <c r="D15" s="154" t="str">
+      <c r="C15" s="158"/>
+      <c r="D15" s="160" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="154"/>
-      <c r="F15" s="154"/>
-      <c r="G15" s="154"/>
-      <c r="H15" s="154"/>
-      <c r="I15" s="154"/>
-      <c r="J15" s="154"/>
-      <c r="K15" s="154"/>
+      <c r="E15" s="160"/>
+      <c r="F15" s="160"/>
+      <c r="G15" s="160"/>
+      <c r="H15" s="160"/>
+      <c r="I15" s="160"/>
+      <c r="J15" s="160"/>
+      <c r="K15" s="160"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="155" t="s">
+      <c r="B16" s="158" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="155"/>
-      <c r="D16" s="154" t="str">
+      <c r="C16" s="158"/>
+      <c r="D16" s="160" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 120° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="154"/>
-      <c r="F16" s="154"/>
-      <c r="G16" s="154"/>
-      <c r="H16" s="154"/>
-      <c r="I16" s="154"/>
-      <c r="J16" s="154"/>
-      <c r="K16" s="154"/>
+      <c r="E16" s="160"/>
+      <c r="F16" s="160"/>
+      <c r="G16" s="160"/>
+      <c r="H16" s="160"/>
+      <c r="I16" s="160"/>
+      <c r="J16" s="160"/>
+      <c r="K16" s="160"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="155" t="s">
+      <c r="B17" s="158" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="155"/>
-      <c r="D17" s="154">
+      <c r="C17" s="158"/>
+      <c r="D17" s="160">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="154"/>
-      <c r="F17" s="154"/>
-      <c r="G17" s="154"/>
-      <c r="H17" s="154"/>
-      <c r="I17" s="154"/>
-      <c r="J17" s="154"/>
-      <c r="K17" s="154"/>
+      <c r="E17" s="160"/>
+      <c r="F17" s="160"/>
+      <c r="G17" s="160"/>
+      <c r="H17" s="160"/>
+      <c r="I17" s="160"/>
+      <c r="J17" s="160"/>
+      <c r="K17" s="160"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="155" t="s">
+      <c r="B18" s="158" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="155"/>
-      <c r="D18" s="165">
+      <c r="C18" s="158"/>
+      <c r="D18" s="159">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="165"/>
-      <c r="F18" s="165"/>
-      <c r="G18" s="165"/>
-      <c r="H18" s="165"/>
-      <c r="I18" s="165"/>
-      <c r="J18" s="165"/>
-      <c r="K18" s="165"/>
+      <c r="E18" s="159"/>
+      <c r="F18" s="159"/>
+      <c r="G18" s="159"/>
+      <c r="H18" s="159"/>
+      <c r="I18" s="159"/>
+      <c r="J18" s="159"/>
+      <c r="K18" s="159"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -34101,16 +34072,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="156"/>
-      <c r="C28" s="157"/>
-      <c r="D28" s="157"/>
-      <c r="E28" s="157"/>
-      <c r="F28" s="157"/>
-      <c r="G28" s="157"/>
-      <c r="H28" s="157"/>
-      <c r="I28" s="157"/>
-      <c r="J28" s="157"/>
-      <c r="K28" s="158"/>
+      <c r="B28" s="165"/>
+      <c r="C28" s="166"/>
+      <c r="D28" s="166"/>
+      <c r="E28" s="166"/>
+      <c r="F28" s="166"/>
+      <c r="G28" s="166"/>
+      <c r="H28" s="166"/>
+      <c r="I28" s="166"/>
+      <c r="J28" s="166"/>
+      <c r="K28" s="167"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -38036,6 +38007,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -38049,13 +38027,6 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="18" priority="3" stopIfTrue="1" operator="between">
@@ -38092,12 +38063,12 @@
   <sheetPr codeName="Tabelle12"/>
   <dimension ref="B2:R135"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="21" topLeftCell="B107" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="B6" sqref="B6"/>
       <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
-      <selection pane="bottomRight" activeCell="H36" sqref="H36"/>
+      <selection pane="bottomRight" activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -38212,10 +38183,10 @@
       <c r="L27" s="103" t="s">
         <v>197</v>
       </c>
-      <c r="N27" s="166"/>
-      <c r="O27" s="166"/>
-      <c r="P27" s="166"/>
-      <c r="Q27" s="166"/>
+      <c r="N27" s="104"/>
+      <c r="O27" s="104"/>
+      <c r="P27" s="104"/>
+      <c r="Q27" s="104"/>
       <c r="R27" t="str">
         <f t="shared" ref="R27:R66" si="0">IF(H27&lt;&gt;"",H27,"")</f>
         <v>Simplified formula used, therefore not evaluated</v>
@@ -38254,16 +38225,16 @@
       <c r="M28" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N28" s="167">
+      <c r="N28" s="107">
         <v>153.74071147146736</v>
       </c>
-      <c r="O28" s="167">
+      <c r="O28" s="107">
         <v>153.74071147146736</v>
       </c>
-      <c r="P28" s="167">
+      <c r="P28" s="107">
         <v>153.74071147146736</v>
       </c>
-      <c r="Q28" s="167">
+      <c r="Q28" s="107">
         <v>153.74071147146736</v>
       </c>
       <c r="R28" t="str">
@@ -38302,16 +38273,16 @@
       <c r="M29" s="103" t="s">
         <v>205</v>
       </c>
-      <c r="N29" s="167">
+      <c r="N29" s="107">
         <v>900</v>
       </c>
-      <c r="O29" s="167">
+      <c r="O29" s="107">
         <v>900</v>
       </c>
-      <c r="P29" s="167">
+      <c r="P29" s="107">
         <v>900</v>
       </c>
-      <c r="Q29" s="167">
+      <c r="Q29" s="107">
         <v>900</v>
       </c>
       <c r="R29" t="str">
@@ -38347,16 +38318,16 @@
       <c r="M30" s="103" t="s">
         <v>143</v>
       </c>
-      <c r="N30" s="167">
+      <c r="N30" s="107">
         <v>4344.0716042398344</v>
       </c>
-      <c r="O30" s="167">
+      <c r="O30" s="107">
         <v>4344.0716042398344</v>
       </c>
-      <c r="P30" s="167">
+      <c r="P30" s="107">
         <v>4344.0716042398344</v>
       </c>
-      <c r="Q30" s="167">
+      <c r="Q30" s="107">
         <v>4344.0716042398344</v>
       </c>
       <c r="R30" t="str">
@@ -38401,16 +38372,16 @@
       <c r="M31" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N31" s="167">
+      <c r="N31" s="107">
         <v>2876</v>
       </c>
-      <c r="O31" s="167">
+      <c r="O31" s="107">
         <v>2876</v>
       </c>
-      <c r="P31" s="167">
+      <c r="P31" s="107">
         <v>2876</v>
       </c>
-      <c r="Q31" s="167">
+      <c r="Q31" s="107">
         <v>2876</v>
       </c>
       <c r="R31" t="str">
@@ -38442,16 +38413,16 @@
       <c r="M32" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N32" s="167">
+      <c r="N32" s="107">
         <v>3144.2390271487925</v>
       </c>
-      <c r="O32" s="167">
+      <c r="O32" s="107">
         <v>3144.2390271487925</v>
       </c>
-      <c r="P32" s="167">
+      <c r="P32" s="107">
         <v>3144.2390271487925</v>
       </c>
-      <c r="Q32" s="167">
+      <c r="Q32" s="107">
         <v>3144.2390271487925</v>
       </c>
       <c r="R32" t="str">
@@ -38483,16 +38454,16 @@
       <c r="M33" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N33" s="169">
+      <c r="N33" s="109">
         <v>0.03</v>
       </c>
-      <c r="O33" s="169">
+      <c r="O33" s="109">
         <v>0.03</v>
       </c>
-      <c r="P33" s="169">
+      <c r="P33" s="109">
         <v>0.03</v>
       </c>
-      <c r="Q33" s="169">
+      <c r="Q33" s="109">
         <v>0.03</v>
       </c>
       <c r="R33" t="str">
@@ -38527,16 +38498,16 @@
       <c r="M34" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N34" s="167">
+      <c r="N34" s="107">
         <v>3074.8142294293471</v>
       </c>
-      <c r="O34" s="167">
+      <c r="O34" s="107">
         <v>3074.8142294293471</v>
       </c>
-      <c r="P34" s="167">
+      <c r="P34" s="107">
         <v>3074.8142294293471</v>
       </c>
-      <c r="Q34" s="167">
+      <c r="Q34" s="107">
         <v>3074.8142294293471</v>
       </c>
       <c r="R34" t="str">
@@ -38578,16 +38549,16 @@
       <c r="M35" s="130" t="s">
         <v>127</v>
       </c>
-      <c r="N35" s="176">
+      <c r="N35" s="129">
         <v>2872.2135022516127</v>
       </c>
-      <c r="O35" s="176">
+      <c r="O35" s="129">
         <v>2872.2135022516127</v>
       </c>
-      <c r="P35" s="176">
+      <c r="P35" s="129">
         <v>2872.2135022516127</v>
       </c>
-      <c r="Q35" s="176">
+      <c r="Q35" s="129">
         <v>2872.2135022516127</v>
       </c>
       <c r="R35" t="str">
@@ -38624,16 +38595,16 @@
       <c r="M36" s="103" t="s">
         <v>275</v>
       </c>
-      <c r="N36" s="174">
+      <c r="N36" s="114">
         <v>5.8458922294713925E-10</v>
       </c>
-      <c r="O36" s="174">
+      <c r="O36" s="114">
         <v>5.8458922294713925E-10</v>
       </c>
-      <c r="P36" s="174">
+      <c r="P36" s="114">
         <v>5.8458922294713925E-10</v>
       </c>
-      <c r="Q36" s="174">
+      <c r="Q36" s="114">
         <v>5.8458922294713925E-10</v>
       </c>
       <c r="R36" t="str">
@@ -38671,16 +38642,16 @@
       <c r="M37" s="103" t="s">
         <v>275</v>
       </c>
-      <c r="N37" s="174">
+      <c r="N37" s="114">
         <v>9.6993208304588435E-11</v>
       </c>
-      <c r="O37" s="174">
+      <c r="O37" s="114">
         <v>9.6993208304588435E-11</v>
       </c>
-      <c r="P37" s="174">
+      <c r="P37" s="114">
         <v>9.6993208304588435E-11</v>
       </c>
-      <c r="Q37" s="174">
+      <c r="Q37" s="114">
         <v>9.6993208304588435E-11</v>
       </c>
       <c r="R37" t="str">
@@ -38718,16 +38689,16 @@
       <c r="M38" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N38" s="169">
+      <c r="N38" s="109">
         <v>0.1423059102718657</v>
       </c>
-      <c r="O38" s="169">
+      <c r="O38" s="109">
         <v>0.1423059102718657</v>
       </c>
-      <c r="P38" s="169">
+      <c r="P38" s="109">
         <v>0.1423059102718657</v>
       </c>
-      <c r="Q38" s="169">
+      <c r="Q38" s="109">
         <v>0.1423059102718657</v>
       </c>
       <c r="R38" t="str">
@@ -38766,16 +38737,16 @@
       <c r="M39" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N39" s="168">
+      <c r="N39" s="108">
         <v>48.860015706266829</v>
       </c>
-      <c r="O39" s="168">
+      <c r="O39" s="108">
         <v>48.860015706266829</v>
       </c>
-      <c r="P39" s="168">
+      <c r="P39" s="108">
         <v>48.860015706266829</v>
       </c>
-      <c r="Q39" s="168">
+      <c r="Q39" s="108">
         <v>48.860015706266829</v>
       </c>
       <c r="R39" t="str">
@@ -38808,16 +38779,16 @@
       <c r="M40" s="103" t="s">
         <v>274</v>
       </c>
-      <c r="N40" s="167">
+      <c r="N40" s="107">
         <v>500</v>
       </c>
-      <c r="O40" s="167">
+      <c r="O40" s="107">
         <v>500</v>
       </c>
-      <c r="P40" s="167">
+      <c r="P40" s="107">
         <v>500</v>
       </c>
-      <c r="Q40" s="167">
+      <c r="Q40" s="107">
         <v>500</v>
       </c>
       <c r="R40" t="str">
@@ -38859,16 +38830,16 @@
       <c r="M41" s="103" t="s">
         <v>274</v>
       </c>
-      <c r="N41" s="167">
+      <c r="N41" s="107">
         <v>33.30212829607494</v>
       </c>
-      <c r="O41" s="167">
+      <c r="O41" s="107">
         <v>33.30212829607494</v>
       </c>
-      <c r="P41" s="167">
+      <c r="P41" s="107">
         <v>33.30212829607494</v>
       </c>
-      <c r="Q41" s="167">
+      <c r="Q41" s="107">
         <v>33.30212829607494</v>
       </c>
       <c r="R41" t="str">
@@ -38907,16 +38878,16 @@
       <c r="M42" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N42" s="171">
+      <c r="N42" s="111">
         <v>3323.2147772434732</v>
       </c>
-      <c r="O42" s="171">
+      <c r="O42" s="111">
         <v>3323.2147772434732</v>
       </c>
-      <c r="P42" s="171">
+      <c r="P42" s="111">
         <v>3323.2147772434732</v>
       </c>
-      <c r="Q42" s="171">
+      <c r="Q42" s="111">
         <v>3323.2147772434732</v>
       </c>
       <c r="R42" t="str">
@@ -38958,16 +38929,16 @@
       <c r="M43" s="103" t="s">
         <v>183</v>
       </c>
-      <c r="N43" s="167">
+      <c r="N43" s="107">
         <v>321.69549999999998</v>
       </c>
-      <c r="O43" s="167">
+      <c r="O43" s="107">
         <v>321.69549999999998</v>
       </c>
-      <c r="P43" s="167">
+      <c r="P43" s="107">
         <v>321.69549999999998</v>
       </c>
-      <c r="Q43" s="167">
+      <c r="Q43" s="107">
         <v>321.69549999999998</v>
       </c>
       <c r="R43" t="str">
@@ -39006,16 +38977,16 @@
       <c r="M44" s="103" t="s">
         <v>183</v>
       </c>
-      <c r="N44" s="167">
+      <c r="N44" s="107">
         <v>321.69549999999998</v>
       </c>
-      <c r="O44" s="167">
+      <c r="O44" s="107">
         <v>321.69549999999998</v>
       </c>
-      <c r="P44" s="167">
+      <c r="P44" s="107">
         <v>321.69549999999998</v>
       </c>
-      <c r="Q44" s="167">
+      <c r="Q44" s="107">
         <v>321.69549999999998</v>
       </c>
       <c r="R44" t="str">
@@ -39054,16 +39025,16 @@
       <c r="M45" s="103" t="s">
         <v>183</v>
       </c>
-      <c r="N45" s="167">
+      <c r="N45" s="107">
         <v>-318.4495</v>
       </c>
-      <c r="O45" s="167">
+      <c r="O45" s="107">
         <v>-318.4495</v>
       </c>
-      <c r="P45" s="167">
+      <c r="P45" s="107">
         <v>-318.4495</v>
       </c>
-      <c r="Q45" s="167">
+      <c r="Q45" s="107">
         <v>-318.4495</v>
       </c>
       <c r="R45" t="str">
@@ -39096,16 +39067,16 @@
       <c r="M46" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N46" s="171">
+      <c r="N46" s="111">
         <v>1320.1892068208026</v>
       </c>
-      <c r="O46" s="171">
+      <c r="O46" s="111">
         <v>1320.1892068208026</v>
       </c>
-      <c r="P46" s="171">
+      <c r="P46" s="111">
         <v>1320.1892068208026</v>
       </c>
-      <c r="Q46" s="171">
+      <c r="Q46" s="111">
         <v>1320.1892068208026</v>
       </c>
       <c r="R46" t="str">
@@ -39144,10 +39115,10 @@
       <c r="M47" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N47" s="166"/>
-      <c r="O47" s="166"/>
-      <c r="P47" s="166"/>
-      <c r="Q47" s="166"/>
+      <c r="N47" s="104"/>
+      <c r="O47" s="104"/>
+      <c r="P47" s="104"/>
+      <c r="Q47" s="104"/>
       <c r="R47" t="str">
         <f t="shared" si="0"/>
         <v>(valid in case L-Flange is calculated)</v>
@@ -39182,16 +39153,16 @@
       <c r="M48" s="103" t="s">
         <v>179</v>
       </c>
-      <c r="N48" s="170">
+      <c r="N48" s="110">
         <v>30</v>
       </c>
-      <c r="O48" s="170">
+      <c r="O48" s="110">
         <v>60</v>
       </c>
-      <c r="P48" s="170">
+      <c r="P48" s="110">
         <v>90</v>
       </c>
-      <c r="Q48" s="170">
+      <c r="Q48" s="110">
         <v>120</v>
       </c>
       <c r="R48" t="str">
@@ -39231,16 +39202,16 @@
       <c r="M49" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="N49" s="169">
+      <c r="N49" s="109">
         <v>1.9634954084936207</v>
       </c>
-      <c r="O49" s="169">
+      <c r="O49" s="109">
         <v>3.9269908169872414</v>
       </c>
-      <c r="P49" s="169">
+      <c r="P49" s="109">
         <v>5.8904862254808625</v>
       </c>
-      <c r="Q49" s="169">
+      <c r="Q49" s="109">
         <v>7.8539816339744828</v>
       </c>
       <c r="R49" t="str">
@@ -39277,16 +39248,16 @@
       <c r="M50" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="N50" s="169">
+      <c r="N50" s="109">
         <v>7.5</v>
       </c>
-      <c r="O50" s="169">
+      <c r="O50" s="109">
         <v>7.5</v>
       </c>
-      <c r="P50" s="169">
+      <c r="P50" s="109">
         <v>7.5</v>
       </c>
-      <c r="Q50" s="169">
+      <c r="Q50" s="109">
         <v>7.5</v>
       </c>
       <c r="R50" t="str">
@@ -39323,16 +39294,16 @@
       <c r="M51" s="103" t="s">
         <v>176</v>
       </c>
-      <c r="N51" s="168">
+      <c r="N51" s="108">
         <v>1.4</v>
       </c>
-      <c r="O51" s="168">
+      <c r="O51" s="108">
         <v>1.4</v>
       </c>
-      <c r="P51" s="168">
+      <c r="P51" s="108">
         <v>1.4</v>
       </c>
-      <c r="Q51" s="168">
+      <c r="Q51" s="108">
         <v>1.4</v>
       </c>
       <c r="R51" t="str">
@@ -39375,16 +39346,16 @@
       <c r="M52" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N52" s="169">
+      <c r="N52" s="109">
         <v>0.28773533056547307</v>
       </c>
-      <c r="O52" s="169">
+      <c r="O52" s="109">
         <v>0.74253427729521915</v>
       </c>
-      <c r="P52" s="169">
+      <c r="P52" s="109">
         <v>1.3643968401892383</v>
       </c>
-      <c r="Q52" s="169">
+      <c r="Q52" s="109">
         <v>2.1533230192475301</v>
       </c>
       <c r="R52" t="str">
@@ -39427,16 +39398,16 @@
       <c r="M53" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N53" s="169">
+      <c r="N53" s="109">
         <v>1.2162355202035975</v>
       </c>
-      <c r="O53" s="169">
+      <c r="O53" s="109">
         <v>0.63575115537527993</v>
       </c>
-      <c r="P53" s="169">
+      <c r="P53" s="109">
         <v>0.4993626397773579</v>
       </c>
-      <c r="Q53" s="169">
+      <c r="Q53" s="109">
         <v>0.44426272750754409</v>
       </c>
       <c r="R53" t="str">
@@ -39469,16 +39440,16 @@
       <c r="M54" s="103" t="s">
         <v>172</v>
       </c>
-      <c r="N54" s="169">
+      <c r="N54" s="109">
         <v>1.9634954084936205</v>
       </c>
-      <c r="O54" s="169">
+      <c r="O54" s="109">
         <v>1.9634954084936205</v>
       </c>
-      <c r="P54" s="169">
+      <c r="P54" s="109">
         <v>1.9634954084936205</v>
       </c>
-      <c r="Q54" s="169">
+      <c r="Q54" s="109">
         <v>1.9634954084936205</v>
       </c>
       <c r="R54" t="str">
@@ -39517,16 +39488,16 @@
       <c r="M55" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N55" s="169">
+      <c r="N55" s="109">
         <v>1.9617469257392748</v>
       </c>
-      <c r="O55" s="169">
+      <c r="O55" s="109">
         <v>1.9617469257392748</v>
       </c>
-      <c r="P55" s="169">
+      <c r="P55" s="109">
         <v>1.9617469257392748</v>
       </c>
-      <c r="Q55" s="169">
+      <c r="Q55" s="109">
         <v>1.9617469257392748</v>
       </c>
       <c r="R55" t="str">
@@ -39565,16 +39536,16 @@
       <c r="M56" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N56" s="169">
+      <c r="N56" s="109">
         <v>2.942620388608912</v>
       </c>
-      <c r="O56" s="169">
+      <c r="O56" s="109">
         <v>2.942620388608912</v>
       </c>
-      <c r="P56" s="169">
+      <c r="P56" s="109">
         <v>2.942620388608912</v>
       </c>
-      <c r="Q56" s="169">
+      <c r="Q56" s="109">
         <v>2.942620388608912</v>
       </c>
       <c r="R56" t="str">
@@ -39609,16 +39580,16 @@
         <v>169</v>
       </c>
       <c r="M57" s="103"/>
-      <c r="N57" s="169">
+      <c r="N57" s="109">
         <v>0.95286282352314688</v>
       </c>
-      <c r="O57" s="169">
+      <c r="O57" s="109">
         <v>0.58262609700472079</v>
       </c>
-      <c r="P57" s="169">
+      <c r="P57" s="109">
         <v>0.47184092472685457</v>
       </c>
-      <c r="Q57" s="169">
+      <c r="Q57" s="109">
         <v>0.42441366570439232</v>
       </c>
       <c r="R57" t="str">
@@ -39653,16 +39624,16 @@
         <v>168</v>
       </c>
       <c r="M58" s="103"/>
-      <c r="N58" s="169">
+      <c r="N58" s="109">
         <v>-1.6996879926957522</v>
       </c>
-      <c r="O58" s="169">
+      <c r="O58" s="109">
         <v>-0.46741282911895099</v>
       </c>
-      <c r="P58" s="169">
+      <c r="P58" s="109">
         <v>0.19939552653846943</v>
       </c>
-      <c r="Q58" s="169">
+      <c r="Q58" s="109">
         <v>0.67694875947348121</v>
       </c>
       <c r="R58" t="str">
@@ -39697,16 +39668,16 @@
         <v>167</v>
       </c>
       <c r="M59" s="103"/>
-      <c r="N59" s="169">
+      <c r="N59" s="109">
         <v>-0.13232393428252798</v>
       </c>
-      <c r="O59" s="169">
+      <c r="O59" s="109">
         <v>0.49094883784411425</v>
       </c>
-      <c r="P59" s="169">
+      <c r="P59" s="109">
         <v>0.97552666362167262</v>
       </c>
-      <c r="Q59" s="169">
+      <c r="Q59" s="109">
         <v>1.3750667981906362</v>
       </c>
       <c r="R59" t="str">
@@ -39749,16 +39720,16 @@
       <c r="M60" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N60" s="169">
+      <c r="N60" s="109">
         <v>0.87601845454409977</v>
       </c>
-      <c r="O60" s="169">
+      <c r="O60" s="109">
         <v>1.6338216149415525</v>
       </c>
-      <c r="P60" s="169">
+      <c r="P60" s="109">
         <v>2.6525058127308667</v>
       </c>
-      <c r="Q60" s="169">
+      <c r="Q60" s="109">
         <v>3.9552630780086151</v>
       </c>
       <c r="R60" t="str">
@@ -39798,16 +39769,16 @@
       <c r="M61" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N61" s="169">
+      <c r="N61" s="109">
         <v>0.87601845454409977</v>
       </c>
-      <c r="O61" s="169">
+      <c r="O61" s="109">
         <v>1.6338216149415525</v>
       </c>
-      <c r="P61" s="169">
+      <c r="P61" s="109">
         <v>2.6525058127308667</v>
       </c>
-      <c r="Q61" s="169">
+      <c r="Q61" s="109">
         <v>3.9552630780086151</v>
       </c>
       <c r="R61" t="str">
@@ -39840,10 +39811,10 @@
         <v>163</v>
       </c>
       <c r="M62" s="103"/>
-      <c r="N62" s="175"/>
-      <c r="O62" s="175"/>
-      <c r="P62" s="175"/>
-      <c r="Q62" s="175"/>
+      <c r="N62" s="128"/>
+      <c r="O62" s="128"/>
+      <c r="P62" s="128"/>
+      <c r="Q62" s="128"/>
       <c r="R62" t="str">
         <f t="shared" si="0"/>
         <v>Gap shape formula</v>
@@ -39874,10 +39845,10 @@
         <v>161</v>
       </c>
       <c r="M63" s="103"/>
-      <c r="N63" s="175"/>
-      <c r="O63" s="175"/>
-      <c r="P63" s="175"/>
-      <c r="Q63" s="175"/>
+      <c r="N63" s="128"/>
+      <c r="O63" s="128"/>
+      <c r="P63" s="128"/>
+      <c r="Q63" s="128"/>
       <c r="R63" t="str">
         <f t="shared" si="0"/>
         <v>Stress range formula</v>
@@ -39905,10 +39876,10 @@
         <v>159</v>
       </c>
       <c r="M64" s="103"/>
-      <c r="N64" s="166"/>
-      <c r="O64" s="166"/>
-      <c r="P64" s="166"/>
-      <c r="Q64" s="166"/>
+      <c r="N64" s="104"/>
+      <c r="O64" s="104"/>
+      <c r="P64" s="104"/>
+      <c r="Q64" s="104"/>
       <c r="R64" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -39936,10 +39907,10 @@
         <v>158</v>
       </c>
       <c r="M65" s="103"/>
-      <c r="N65" s="166"/>
-      <c r="O65" s="166"/>
-      <c r="P65" s="166"/>
-      <c r="Q65" s="166"/>
+      <c r="N65" s="104"/>
+      <c r="O65" s="104"/>
+      <c r="P65" s="104"/>
+      <c r="Q65" s="104"/>
       <c r="R65" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -39970,10 +39941,10 @@
         <v>157</v>
       </c>
       <c r="M66" s="103"/>
-      <c r="N66" s="175"/>
-      <c r="O66" s="175"/>
-      <c r="P66" s="175"/>
-      <c r="Q66" s="175"/>
+      <c r="N66" s="128"/>
+      <c r="O66" s="128"/>
+      <c r="P66" s="128"/>
+      <c r="Q66" s="128"/>
       <c r="R66" t="str">
         <f t="shared" si="0"/>
         <v>Summarized formula for bolt force curve</v>
@@ -40006,16 +39977,16 @@
       <c r="M67" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N67" s="169">
+      <c r="N67" s="109">
         <v>-123.29166666666667</v>
       </c>
-      <c r="O67" s="169">
+      <c r="O67" s="109">
         <v>-123.29166666666667</v>
       </c>
-      <c r="P67" s="169">
+      <c r="P67" s="109">
         <v>-123.29166666666667</v>
       </c>
-      <c r="Q67" s="169">
+      <c r="Q67" s="109">
         <v>-123.29166666666667</v>
       </c>
     </row>
@@ -40046,16 +40017,16 @@
       <c r="M68" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N68" s="169">
+      <c r="N68" s="109">
         <v>2876</v>
       </c>
-      <c r="O68" s="169">
+      <c r="O68" s="109">
         <v>2876</v>
       </c>
-      <c r="P68" s="169">
+      <c r="P68" s="109">
         <v>2876</v>
       </c>
-      <c r="Q68" s="169">
+      <c r="Q68" s="109">
         <v>2876</v>
       </c>
     </row>
@@ -40086,16 +40057,16 @@
       <c r="M69" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N69" s="169">
+      <c r="N69" s="109">
         <v>2005.9791663249318</v>
       </c>
-      <c r="O69" s="169">
+      <c r="O69" s="109">
         <v>1698.4770142338571</v>
       </c>
-      <c r="P69" s="169">
+      <c r="P69" s="109">
         <v>1595.9900029492692</v>
       </c>
-      <c r="Q69" s="169">
+      <c r="Q69" s="109">
         <v>1541.0054120283587</v>
       </c>
     </row>
@@ -40126,16 +40097,16 @@
       <c r="M70" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N70" s="169">
+      <c r="N70" s="109">
         <v>3738.8</v>
       </c>
-      <c r="O70" s="169">
+      <c r="O70" s="109">
         <v>3738.8</v>
       </c>
-      <c r="P70" s="169">
+      <c r="P70" s="109">
         <v>3738.8</v>
       </c>
-      <c r="Q70" s="169">
+      <c r="Q70" s="109">
         <v>3738.8</v>
       </c>
     </row>
@@ -40166,16 +40137,16 @@
       <c r="M71" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N71" s="169">
+      <c r="N71" s="109">
         <v>244.94742536995892</v>
       </c>
-      <c r="O71" s="169">
+      <c r="O71" s="109">
         <v>138.78694642015648</v>
       </c>
-      <c r="P71" s="169">
+      <c r="P71" s="109">
         <v>121.65181485180494</v>
       </c>
-      <c r="Q71" s="169">
+      <c r="Q71" s="109">
         <v>114.92158217798261</v>
       </c>
     </row>
@@ -40206,16 +40177,16 @@
       <c r="M72" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N72" s="169">
+      <c r="N72" s="109">
         <v>2929.4096341509371</v>
       </c>
-      <c r="O72" s="169">
+      <c r="O72" s="109">
         <v>2900.9817597314391</v>
       </c>
-      <c r="P72" s="169">
+      <c r="P72" s="109">
         <v>2896.6973875621416</v>
       </c>
-      <c r="Q72" s="169">
+      <c r="Q72" s="109">
         <v>2895.2807275311129</v>
       </c>
     </row>
@@ -40238,16 +40209,16 @@
         <v>309</v>
       </c>
       <c r="M73" s="103"/>
-      <c r="N73" s="170">
+      <c r="N73" s="110">
         <v>1380791102.7342598</v>
       </c>
-      <c r="O73" s="170">
+      <c r="O73" s="110">
         <v>744668734.36700821</v>
       </c>
-      <c r="P73" s="170">
+      <c r="P73" s="110">
         <v>620883379.09948421</v>
       </c>
-      <c r="Q73" s="170">
+      <c r="Q73" s="110">
         <v>565381792.77264023</v>
       </c>
     </row>
@@ -40270,16 +40241,16 @@
         <v>308</v>
       </c>
       <c r="M74" s="103"/>
-      <c r="N74" s="171">
+      <c r="N74" s="111">
         <v>203993.11241085827</v>
       </c>
-      <c r="O74" s="171">
+      <c r="O74" s="111">
         <v>180610.43989879353</v>
       </c>
-      <c r="P74" s="171">
+      <c r="P74" s="111">
         <v>175752.59680961052</v>
       </c>
-      <c r="Q74" s="171">
+      <c r="Q74" s="111">
         <v>173441.53259801748</v>
       </c>
     </row>
@@ -40302,16 +40273,16 @@
         <v>307</v>
       </c>
       <c r="M75" s="103"/>
-      <c r="N75" s="171">
+      <c r="N75" s="111">
         <v>175453890.51960349</v>
       </c>
-      <c r="O75" s="171">
+      <c r="O75" s="111">
         <v>68184425.844646752</v>
       </c>
-      <c r="P75" s="171">
+      <c r="P75" s="111">
         <v>52752000.46785488</v>
       </c>
-      <c r="Q75" s="171">
+      <c r="Q75" s="111">
         <v>47213122.514237635</v>
       </c>
     </row>
@@ -40338,16 +40309,16 @@
         <v>306</v>
       </c>
       <c r="M76" s="103"/>
-      <c r="N76" s="178">
+      <c r="N76" s="154">
         <v>1.4773640415766625E-4</v>
       </c>
-      <c r="O76" s="178">
+      <c r="O76" s="154">
         <v>2.4253796562617613E-4</v>
       </c>
-      <c r="P76" s="178">
+      <c r="P76" s="154">
         <v>2.8306861276350848E-4</v>
       </c>
-      <c r="Q76" s="178">
+      <c r="Q76" s="154">
         <v>3.0676886807312593E-4</v>
       </c>
     </row>
@@ -40374,16 +40345,16 @@
         <v>305</v>
       </c>
       <c r="M77" s="103"/>
-      <c r="N77" s="178">
+      <c r="N77" s="154">
         <v>0.12706765720909374</v>
       </c>
-      <c r="O77" s="178">
+      <c r="O77" s="154">
         <v>9.1563433105064707E-2</v>
       </c>
-      <c r="P77" s="178">
+      <c r="P77" s="154">
         <v>8.4962816276971748E-2</v>
       </c>
-      <c r="Q77" s="178">
+      <c r="Q77" s="154">
         <v>8.3506619982762126E-2</v>
       </c>
     </row>
@@ -40410,16 +40381,16 @@
         <v>304</v>
       </c>
       <c r="M78" s="103"/>
-      <c r="N78" s="168">
+      <c r="N78" s="108">
         <v>2889.4206665233846</v>
       </c>
-      <c r="O78" s="168">
+      <c r="O78" s="108">
         <v>2883.6022286596831</v>
       </c>
-      <c r="P78" s="168">
+      <c r="P78" s="108">
         <v>2882.172327927527</v>
       </c>
-      <c r="Q78" s="168">
+      <c r="Q78" s="108">
         <v>2881.6325273873549</v>
       </c>
     </row>
@@ -40457,16 +40428,16 @@
       <c r="M79" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N79" s="167">
+      <c r="N79" s="107">
         <v>1221.3620300054099</v>
       </c>
-      <c r="O79" s="167">
+      <c r="O79" s="107">
         <v>802.68684894274077</v>
       </c>
-      <c r="P79" s="167">
+      <c r="P79" s="107">
         <v>711.5482385942081</v>
       </c>
-      <c r="Q79" s="167">
+      <c r="Q79" s="107">
         <v>681.5727326421669</v>
       </c>
       <c r="R79" t="str">
@@ -40498,16 +40469,16 @@
       <c r="M80" s="103" t="s">
         <v>143</v>
       </c>
-      <c r="N80" s="171">
+      <c r="N80" s="111">
         <v>38819.613222857879</v>
       </c>
-      <c r="O80" s="171">
+      <c r="O80" s="111">
         <v>38819.613222857879</v>
       </c>
-      <c r="P80" s="171">
+      <c r="P80" s="111">
         <v>38819.613222857879</v>
       </c>
-      <c r="Q80" s="171">
+      <c r="Q80" s="111">
         <v>38819.613222857879</v>
       </c>
       <c r="R80" t="str">
@@ -40543,16 +40514,16 @@
       <c r="M81" s="103" t="s">
         <v>273</v>
       </c>
-      <c r="N81" s="177">
+      <c r="N81" s="153">
         <v>129398710.7428596</v>
       </c>
-      <c r="O81" s="177">
+      <c r="O81" s="153">
         <v>129398710.7428596</v>
       </c>
-      <c r="P81" s="177">
+      <c r="P81" s="153">
         <v>129398710.7428596</v>
       </c>
-      <c r="Q81" s="177">
+      <c r="Q81" s="153">
         <v>129398710.7428596</v>
       </c>
       <c r="R81" t="str">
@@ -40588,16 +40559,16 @@
       <c r="M82" s="103" t="s">
         <v>143</v>
       </c>
-      <c r="N82" s="171">
+      <c r="N82" s="111">
         <v>87000</v>
       </c>
-      <c r="O82" s="171">
+      <c r="O82" s="111">
         <v>87000</v>
       </c>
-      <c r="P82" s="171">
+      <c r="P82" s="111">
         <v>87000</v>
       </c>
-      <c r="Q82" s="171">
+      <c r="Q82" s="111">
         <v>87000</v>
       </c>
       <c r="R82" t="str">
@@ -40633,16 +40604,16 @@
       <c r="M83" s="103" t="s">
         <v>273</v>
       </c>
-      <c r="N83" s="177">
+      <c r="N83" s="153">
         <v>290000000</v>
       </c>
-      <c r="O83" s="177">
+      <c r="O83" s="153">
         <v>290000000</v>
       </c>
-      <c r="P83" s="177">
+      <c r="P83" s="153">
         <v>290000000</v>
       </c>
-      <c r="Q83" s="177">
+      <c r="Q83" s="153">
         <v>290000000</v>
       </c>
       <c r="R83" t="str">
@@ -40684,16 +40655,16 @@
       <c r="M84" s="103" t="s">
         <v>134</v>
       </c>
-      <c r="N84" s="171">
+      <c r="N84" s="111">
         <v>14366.135107106511</v>
       </c>
-      <c r="O84" s="171">
+      <c r="O84" s="111">
         <v>5062.3281975086429</v>
       </c>
-      <c r="P84" s="171">
+      <c r="P84" s="111">
         <v>2764.1193483222332</v>
       </c>
-      <c r="Q84" s="171">
+      <c r="Q84" s="111">
         <v>1775.6019758133866</v>
       </c>
       <c r="R84" t="str">
@@ -40734,16 +40705,16 @@
       <c r="M85" s="103" t="s">
         <v>134</v>
       </c>
-      <c r="N85" s="171">
+      <c r="N85" s="111">
         <v>4747.6491403977416</v>
       </c>
-      <c r="O85" s="171">
+      <c r="O85" s="111">
         <v>1990.4379337589339</v>
       </c>
-      <c r="P85" s="171">
+      <c r="P85" s="111">
         <v>1050.2469446066798</v>
       </c>
-      <c r="Q85" s="171">
+      <c r="Q85" s="111">
         <v>591.4518990117981</v>
       </c>
       <c r="R85" t="str">
@@ -40782,16 +40753,16 @@
       <c r="M86" s="103" t="s">
         <v>134</v>
       </c>
-      <c r="N86" s="171">
+      <c r="N86" s="111">
         <v>5109.9347062037868</v>
       </c>
-      <c r="O86" s="171">
+      <c r="O86" s="111">
         <v>2205.3060735850058</v>
       </c>
-      <c r="P86" s="171">
+      <c r="P86" s="111">
         <v>1237.2237731143939</v>
       </c>
-      <c r="Q86" s="171">
+      <c r="Q86" s="111">
         <v>800.98702799963189</v>
       </c>
       <c r="R86" t="str">
@@ -40830,16 +40801,16 @@
       <c r="M87" s="103" t="s">
         <v>134</v>
       </c>
-      <c r="N87" s="171">
+      <c r="N87" s="111">
         <v>5109.9347062037868</v>
       </c>
-      <c r="O87" s="171">
+      <c r="O87" s="111">
         <v>2205.3060735850058</v>
       </c>
-      <c r="P87" s="171">
+      <c r="P87" s="111">
         <v>1237.2237731143939</v>
       </c>
-      <c r="Q87" s="171">
+      <c r="Q87" s="111">
         <v>800.98702799963189</v>
       </c>
       <c r="R87" t="str">
@@ -40881,16 +40852,16 @@
       <c r="M88" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N88" s="169">
+      <c r="N88" s="109">
         <v>1.8</v>
       </c>
-      <c r="O88" s="169">
+      <c r="O88" s="109">
         <v>2.0853981633974481</v>
       </c>
-      <c r="P88" s="169">
+      <c r="P88" s="109">
         <v>2.4780972450961727</v>
       </c>
-      <c r="Q88" s="169">
+      <c r="Q88" s="109">
         <v>2.8707963267948964</v>
       </c>
       <c r="R88" t="str">
@@ -40932,16 +40903,16 @@
       <c r="M89" s="103" t="s">
         <v>134</v>
       </c>
-      <c r="N89" s="167">
+      <c r="N89" s="107">
         <v>1420.1267061173537</v>
       </c>
-      <c r="O89" s="167">
+      <c r="O89" s="107">
         <v>95.752198009831758</v>
       </c>
-      <c r="P89" s="167">
+      <c r="P89" s="107">
         <v>19.194112486621197</v>
       </c>
-      <c r="Q89" s="167">
+      <c r="Q89" s="107">
         <v>6.104779188271074</v>
       </c>
       <c r="R89" t="str">
@@ -40982,16 +40953,16 @@
       <c r="M90" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N90" s="167">
+      <c r="N90" s="107">
         <v>550.90080499035628</v>
       </c>
-      <c r="O90" s="167">
+      <c r="O90" s="107">
         <v>572.58710847833606</v>
       </c>
-      <c r="P90" s="167">
+      <c r="P90" s="107">
         <v>577.99584146472671</v>
       </c>
-      <c r="Q90" s="167">
+      <c r="Q90" s="107">
         <v>579.568707746938</v>
       </c>
       <c r="R90" t="str">
@@ -41032,16 +41003,16 @@
       <c r="M91" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N91" s="167">
+      <c r="N91" s="107">
         <v>426.11545542928133</v>
       </c>
-      <c r="O91" s="167">
+      <c r="O91" s="107">
         <v>329.67533542437053</v>
       </c>
-      <c r="P91" s="167">
+      <c r="P91" s="107">
         <v>305.62241840367358</v>
       </c>
-      <c r="Q91" s="167">
+      <c r="Q91" s="107">
         <v>298.62780020642253</v>
       </c>
       <c r="R91" t="str">
@@ -41081,16 +41052,16 @@
       <c r="M92" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N92" s="168">
+      <c r="N92" s="108">
         <v>0</v>
       </c>
-      <c r="O92" s="168">
+      <c r="O92" s="108">
         <v>0</v>
       </c>
-      <c r="P92" s="168">
+      <c r="P92" s="108">
         <v>0</v>
       </c>
-      <c r="Q92" s="168">
+      <c r="Q92" s="108">
         <v>0</v>
       </c>
       <c r="R92" t="str">
@@ -41129,16 +41100,16 @@
       <c r="M93" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N93" s="167">
+      <c r="N93" s="107">
         <v>1221.3620300054099</v>
       </c>
-      <c r="O93" s="167">
+      <c r="O93" s="107">
         <v>802.68684894274077</v>
       </c>
-      <c r="P93" s="167">
+      <c r="P93" s="107">
         <v>711.5482385942081</v>
       </c>
-      <c r="Q93" s="167">
+      <c r="Q93" s="107">
         <v>681.5727326421669</v>
       </c>
       <c r="R93" t="str">
@@ -41176,16 +41147,16 @@
       <c r="M94" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N94" s="167">
+      <c r="N94" s="107">
         <v>3595</v>
       </c>
-      <c r="O94" s="167">
+      <c r="O94" s="107">
         <v>3595</v>
       </c>
-      <c r="P94" s="167">
+      <c r="P94" s="107">
         <v>3595</v>
       </c>
-      <c r="Q94" s="167">
+      <c r="Q94" s="107">
         <v>3595</v>
       </c>
       <c r="R94" t="str">
@@ -41230,16 +41201,16 @@
       <c r="M95" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N95" s="167">
+      <c r="N95" s="107">
         <v>2068.2520235998149</v>
       </c>
-      <c r="O95" s="167">
+      <c r="O95" s="107">
         <v>2068.2520235998149</v>
       </c>
-      <c r="P95" s="167">
+      <c r="P95" s="107">
         <v>2068.2520235998149</v>
       </c>
-      <c r="Q95" s="167">
+      <c r="Q95" s="107">
         <v>2068.2520235998149</v>
       </c>
       <c r="R95" t="str">
@@ -41280,16 +41251,16 @@
       <c r="M96" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N96" s="168">
+      <c r="N96" s="108">
         <v>2068.2520235998149</v>
       </c>
-      <c r="O96" s="168">
+      <c r="O96" s="108">
         <v>2068.2520235998149</v>
       </c>
-      <c r="P96" s="168">
+      <c r="P96" s="108">
         <v>2068.2520235998149</v>
       </c>
-      <c r="Q96" s="168">
+      <c r="Q96" s="108">
         <v>2068.2520235998149</v>
       </c>
       <c r="R96" t="str">
@@ -41331,16 +41302,16 @@
       <c r="M97" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N97" s="169">
+      <c r="N97" s="109">
         <v>2.3686419505455167</v>
       </c>
-      <c r="O97" s="169">
+      <c r="O97" s="109">
         <v>1.3420699686162645</v>
       </c>
-      <c r="P97" s="169">
+      <c r="P97" s="109">
         <v>1.1763732220609038</v>
       </c>
-      <c r="Q97" s="169">
+      <c r="Q97" s="109">
         <v>1.1112918625647985</v>
       </c>
       <c r="R97" t="str">
@@ -41372,16 +41343,16 @@
       <c r="M98" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N98" s="167">
+      <c r="N98" s="107">
         <v>194.0980661142894</v>
       </c>
-      <c r="O98" s="167">
+      <c r="O98" s="107">
         <v>194.0980661142894</v>
       </c>
-      <c r="P98" s="167">
+      <c r="P98" s="107">
         <v>194.0980661142894</v>
       </c>
-      <c r="Q98" s="167">
+      <c r="Q98" s="107">
         <v>194.0980661142894</v>
       </c>
       <c r="R98" t="str">
@@ -41423,16 +41394,16 @@
       <c r="M99" s="103" t="s">
         <v>134</v>
       </c>
-      <c r="N99" s="167">
+      <c r="N99" s="107">
         <v>10496.635077845174</v>
       </c>
-      <c r="O99" s="167">
+      <c r="O99" s="107">
         <v>14799.101534655869</v>
       </c>
-      <c r="P99" s="167">
+      <c r="P99" s="107">
         <v>15671.989863448487</v>
       </c>
-      <c r="Q99" s="167">
+      <c r="Q99" s="107">
         <v>15954.463649842879</v>
       </c>
       <c r="R99" t="str">
@@ -41474,16 +41445,16 @@
       <c r="M100" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N100" s="171">
+      <c r="N100" s="111">
         <v>846.88999359440504</v>
       </c>
-      <c r="O100" s="171">
+      <c r="O100" s="111">
         <v>1265.5651746570743</v>
       </c>
-      <c r="P100" s="171">
+      <c r="P100" s="111">
         <v>1356.7037850056067</v>
       </c>
-      <c r="Q100" s="171">
+      <c r="Q100" s="111">
         <v>1386.6792909576479</v>
       </c>
       <c r="R100" t="str">
@@ -41528,16 +41499,16 @@
       <c r="M101" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N101" s="169">
+      <c r="N101" s="109">
         <v>0.41567671207598361</v>
       </c>
-      <c r="O101" s="169">
+      <c r="O101" s="109">
         <v>0.4405832248256456</v>
       </c>
-      <c r="P101" s="169">
+      <c r="P101" s="109">
         <v>0.44600495762306314</v>
       </c>
-      <c r="Q101" s="169">
+      <c r="Q101" s="109">
         <v>0.44778816655194476</v>
       </c>
       <c r="R101" t="str">
@@ -41576,16 +41547,16 @@
       <c r="M102" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N102" s="169">
+      <c r="N102" s="109">
         <v>0.41567671207598361</v>
       </c>
-      <c r="O102" s="169">
+      <c r="O102" s="109">
         <v>0.4405832248256456</v>
       </c>
-      <c r="P102" s="169">
+      <c r="P102" s="109">
         <v>0.44600495762306314</v>
       </c>
-      <c r="Q102" s="169">
+      <c r="Q102" s="109">
         <v>0.44778816655194476</v>
       </c>
       <c r="R102" t="str">
@@ -41617,16 +41588,16 @@
       <c r="M103" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N103" s="170">
+      <c r="N103" s="110">
         <v>14795</v>
       </c>
-      <c r="O103" s="170">
+      <c r="O103" s="110">
         <v>14795</v>
       </c>
-      <c r="P103" s="170">
+      <c r="P103" s="110">
         <v>14795</v>
       </c>
-      <c r="Q103" s="170">
+      <c r="Q103" s="110">
         <v>14795</v>
       </c>
       <c r="R103" t="str">
@@ -41668,16 +41639,16 @@
       <c r="M104" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N104" s="167">
+      <c r="N104" s="107">
         <v>-123.29166666666667</v>
       </c>
-      <c r="O104" s="167">
+      <c r="O104" s="107">
         <v>-123.29166666666667</v>
       </c>
-      <c r="P104" s="167">
+      <c r="P104" s="107">
         <v>-123.29166666666667</v>
       </c>
-      <c r="Q104" s="167">
+      <c r="Q104" s="107">
         <v>-123.29166666666667</v>
       </c>
       <c r="R104" t="str">
@@ -41699,10 +41670,10 @@
         <v>42</v>
       </c>
       <c r="M105" s="103"/>
-      <c r="N105" s="166"/>
-      <c r="O105" s="166"/>
-      <c r="P105" s="166"/>
-      <c r="Q105" s="166"/>
+      <c r="N105" s="104"/>
+      <c r="O105" s="104"/>
+      <c r="P105" s="104"/>
+      <c r="Q105" s="104"/>
       <c r="R105" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -41742,16 +41713,16 @@
       <c r="M106" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N106" s="167">
+      <c r="N106" s="107">
         <v>-1344.6536966720766</v>
       </c>
-      <c r="O106" s="167">
+      <c r="O106" s="107">
         <v>-925.9785156094074</v>
       </c>
-      <c r="P106" s="167">
+      <c r="P106" s="107">
         <v>-834.83990526087473</v>
       </c>
-      <c r="Q106" s="167">
+      <c r="Q106" s="107">
         <v>-804.86439930883353</v>
       </c>
       <c r="R106" t="str">
@@ -41793,16 +41764,16 @@
       <c r="M107" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N107" s="169">
+      <c r="N107" s="109">
         <v>9.065309586276786E-2</v>
       </c>
-      <c r="O107" s="169">
+      <c r="O107" s="109">
         <v>3.1781866873645398E-2</v>
       </c>
-      <c r="P107" s="169">
+      <c r="P107" s="109">
         <v>1.5191121042335862E-2</v>
       </c>
-      <c r="Q107" s="169">
+      <c r="Q107" s="109">
         <v>7.8932068117869621E-3</v>
       </c>
       <c r="R107" t="str">
@@ -41844,16 +41815,16 @@
       <c r="M108" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N108" s="168">
+      <c r="N108" s="108">
         <v>2820.6398754053871</v>
       </c>
-      <c r="O108" s="168">
+      <c r="O108" s="108">
         <v>2863.2445567128379</v>
       </c>
-      <c r="P108" s="168">
+      <c r="P108" s="108">
         <v>2870.5953922900276</v>
       </c>
-      <c r="Q108" s="168">
+      <c r="Q108" s="108">
         <v>2873.3101027319904</v>
       </c>
       <c r="R108" t="str">
@@ -41898,16 +41869,16 @@
       <c r="M109" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N109" s="173">
+      <c r="N109" s="113">
         <v>0.1450406415449905</v>
       </c>
-      <c r="O109" s="173">
+      <c r="O109" s="113">
         <v>9.5321626733284245E-2</v>
       </c>
-      <c r="P109" s="173">
+      <c r="P109" s="113">
         <v>8.4498625698602059E-2</v>
       </c>
-      <c r="Q109" s="173">
+      <c r="Q109" s="113">
         <v>8.0938938638492219E-2</v>
       </c>
       <c r="R109" t="str">
@@ -41946,16 +41917,16 @@
       <c r="M110" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N110" s="173">
+      <c r="N110" s="113">
         <v>0.1450406415449905</v>
       </c>
-      <c r="O110" s="173">
+      <c r="O110" s="113">
         <v>9.5321626733284245E-2</v>
       </c>
-      <c r="P110" s="173">
+      <c r="P110" s="113">
         <v>8.4498625698602059E-2</v>
       </c>
-      <c r="Q110" s="173">
+      <c r="Q110" s="113">
         <v>8.0938938638492219E-2</v>
       </c>
       <c r="R110" t="str">
@@ -41991,10 +41962,10 @@
       <c r="M111" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N111" s="175"/>
-      <c r="O111" s="175"/>
-      <c r="P111" s="175"/>
-      <c r="Q111" s="175"/>
+      <c r="N111" s="128"/>
+      <c r="O111" s="128"/>
+      <c r="P111" s="128"/>
+      <c r="Q111" s="128"/>
       <c r="R111" t="str">
         <f t="shared" si="6"/>
         <v>Bending moment L-Flange as a function of external force Z</v>
@@ -42034,16 +42005,16 @@
       <c r="M112" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="N112" s="167">
+      <c r="N112" s="107">
         <v>112.77695050276786</v>
       </c>
-      <c r="O112" s="167">
+      <c r="O112" s="107">
         <v>112.77695050276786</v>
       </c>
-      <c r="P112" s="167">
+      <c r="P112" s="107">
         <v>112.77695050276786</v>
       </c>
-      <c r="Q112" s="167">
+      <c r="Q112" s="107">
         <v>112.77695050276786</v>
       </c>
       <c r="R112" t="str">
@@ -42082,16 +42053,16 @@
       <c r="M113" s="103" t="s">
         <v>268</v>
       </c>
-      <c r="N113" s="174">
+      <c r="N113" s="114">
         <v>1.6641565715404047E-9</v>
       </c>
-      <c r="O113" s="174">
+      <c r="O113" s="114">
         <v>1.6641565715404047E-9</v>
       </c>
-      <c r="P113" s="174">
+      <c r="P113" s="114">
         <v>1.6641565715404047E-9</v>
       </c>
-      <c r="Q113" s="174">
+      <c r="Q113" s="114">
         <v>1.6641565715404047E-9</v>
       </c>
       <c r="R113" t="str">
@@ -42127,10 +42098,10 @@
       <c r="M114" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N114" s="175"/>
-      <c r="O114" s="175"/>
-      <c r="P114" s="175"/>
-      <c r="Q114" s="175"/>
+      <c r="N114" s="128"/>
+      <c r="O114" s="128"/>
+      <c r="P114" s="128"/>
+      <c r="Q114" s="128"/>
       <c r="R114" t="str">
         <f t="shared" si="6"/>
         <v>Bending moment for T-Flange as a function of external force Z</v>
@@ -42164,10 +42135,10 @@
       <c r="M115" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N115" s="175"/>
-      <c r="O115" s="175"/>
-      <c r="P115" s="175"/>
-      <c r="Q115" s="175"/>
+      <c r="N115" s="128"/>
+      <c r="O115" s="128"/>
+      <c r="P115" s="128"/>
+      <c r="Q115" s="128"/>
       <c r="R115" t="str">
         <f t="shared" si="6"/>
         <v>Intermediate values as function of Z</v>
@@ -42201,10 +42172,10 @@
       <c r="M116" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N116" s="175"/>
-      <c r="O116" s="175"/>
-      <c r="P116" s="175"/>
-      <c r="Q116" s="175"/>
+      <c r="N116" s="128"/>
+      <c r="O116" s="128"/>
+      <c r="P116" s="128"/>
+      <c r="Q116" s="128"/>
       <c r="R116" t="str">
         <f t="shared" si="6"/>
         <v>Intermediate values as function of Z</v>
@@ -42247,16 +42218,16 @@
       <c r="M117" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N117" s="169">
+      <c r="N117" s="109">
         <v>0.39923954409453227</v>
       </c>
-      <c r="O117" s="169">
+      <c r="O117" s="109">
         <v>0.30526017021619684</v>
       </c>
-      <c r="P117" s="169">
+      <c r="P117" s="109">
         <v>0.28263576272637364</v>
       </c>
-      <c r="Q117" s="169">
+      <c r="Q117" s="109">
         <v>0.27368497967790395</v>
       </c>
       <c r="R117" t="str">
@@ -42290,16 +42261,16 @@
       <c r="M118" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="N118" s="174">
+      <c r="N118" s="114">
         <v>0.24867156308940955</v>
       </c>
-      <c r="O118" s="174">
+      <c r="O118" s="114">
         <v>0.17891343818957089</v>
       </c>
-      <c r="P118" s="174">
+      <c r="P118" s="114">
         <v>0.15639812475964909</v>
       </c>
-      <c r="Q118" s="174">
+      <c r="Q118" s="114">
         <v>0.14764973613876137</v>
       </c>
       <c r="R118" t="str">
@@ -42344,16 +42315,16 @@
       <c r="M119" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N119" s="168">
+      <c r="N119" s="108">
         <v>-258.21702205683982</v>
       </c>
-      <c r="O119" s="168">
+      <c r="O119" s="108">
         <v>-147.9448707371663</v>
       </c>
-      <c r="P119" s="168">
+      <c r="P119" s="108">
         <v>-129.56721252123472</v>
       </c>
-      <c r="Q119" s="168">
+      <c r="Q119" s="108">
         <v>-123.97992500178142</v>
       </c>
       <c r="R119" t="str">
@@ -42387,16 +42358,16 @@
       <c r="M120" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N120" s="168">
+      <c r="N120" s="108">
         <v>-177.46506708584585</v>
       </c>
-      <c r="O120" s="168">
+      <c r="O120" s="108">
         <v>-94.258911259528404</v>
       </c>
-      <c r="P120" s="168">
+      <c r="P120" s="108">
         <v>-77.143193655495082</v>
       </c>
-      <c r="Q120" s="168">
+      <c r="Q120" s="108">
         <v>-71.573212705236273</v>
       </c>
       <c r="R120" t="str">
@@ -42427,16 +42398,16 @@
       <c r="M121" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="N121" s="169">
+      <c r="N121" s="109">
         <v>-123.19166666666668</v>
       </c>
-      <c r="O121" s="169">
+      <c r="O121" s="109">
         <v>-123.19166666666668</v>
       </c>
-      <c r="P121" s="169">
+      <c r="P121" s="109">
         <v>-123.19166666666668</v>
       </c>
-      <c r="Q121" s="169">
+      <c r="Q121" s="109">
         <v>-123.19166666666668</v>
       </c>
     </row>
@@ -42466,16 +42437,16 @@
       <c r="M122" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N122" s="173">
+      <c r="N122" s="113">
         <v>0</v>
       </c>
-      <c r="O122" s="173">
+      <c r="O122" s="113">
         <v>0</v>
       </c>
-      <c r="P122" s="173">
+      <c r="P122" s="113">
         <v>0</v>
       </c>
-      <c r="Q122" s="173">
+      <c r="Q122" s="113">
         <v>0</v>
       </c>
       <c r="R122" s="152" t="s">
@@ -42508,16 +42479,16 @@
       <c r="M123" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N123" s="169">
+      <c r="N123" s="109">
         <v>-71.552154055834237</v>
       </c>
-      <c r="O123" s="169">
+      <c r="O123" s="109">
         <v>-83.756193624864608</v>
       </c>
-      <c r="P123" s="169">
+      <c r="P123" s="109">
         <v>-87.722465386590997</v>
       </c>
-      <c r="Q123" s="169">
+      <c r="Q123" s="109">
         <v>-89.603826344462561</v>
       </c>
       <c r="R123" s="152" t="s">
@@ -42550,16 +42521,16 @@
       <c r="M124" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N124" s="173">
+      <c r="N124" s="113">
         <v>-25.606064536096081</v>
       </c>
-      <c r="O124" s="173">
+      <c r="O124" s="113">
         <v>-22.453179292579161</v>
       </c>
-      <c r="P124" s="173">
+      <c r="P124" s="113">
         <v>-21.500788559412335</v>
       </c>
-      <c r="Q124" s="173">
+      <c r="Q124" s="113">
         <v>-21.256195638241046</v>
       </c>
       <c r="R124" s="152" t="s">
@@ -42592,16 +42563,16 @@
       <c r="M125" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N125" s="173">
+      <c r="N125" s="113">
         <v>9.6452807643820759E-3</v>
       </c>
-      <c r="O125" s="173">
+      <c r="O125" s="113">
         <v>3.3815174903301338E-3</v>
       </c>
-      <c r="P125" s="173">
+      <c r="P125" s="113">
         <v>1.6163003169891762E-3</v>
       </c>
-      <c r="Q125" s="173">
+      <c r="Q125" s="113">
         <v>8.3981903879232667E-4</v>
       </c>
       <c r="R125" s="152" t="s">
@@ -42634,16 +42605,16 @@
       <c r="M126" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N126" s="169">
+      <c r="N126" s="109">
         <v>-71.494119189415173</v>
       </c>
-      <c r="O126" s="169">
+      <c r="O126" s="109">
         <v>-83.688260247135759</v>
       </c>
-      <c r="P126" s="169">
+      <c r="P126" s="109">
         <v>-87.651315026020583</v>
       </c>
-      <c r="Q126" s="169">
+      <c r="Q126" s="109">
         <v>-89.531150040567098</v>
       </c>
       <c r="R126" s="152" t="s">
@@ -42676,16 +42647,16 @@
       <c r="M127" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N127" s="173">
+      <c r="N127" s="113">
         <v>-25.581197379787142</v>
       </c>
-      <c r="O127" s="173">
+      <c r="O127" s="113">
         <v>-22.435287948760205</v>
       </c>
-      <c r="P127" s="173">
+      <c r="P127" s="113">
         <v>-21.485148746936371</v>
       </c>
-      <c r="Q127" s="173">
+      <c r="Q127" s="113">
         <v>-21.24143066462717</v>
       </c>
       <c r="R127" s="152" t="s">
@@ -42715,16 +42686,16 @@
       <c r="M128" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N128" s="168">
+      <c r="N128" s="108">
         <v>-14.409012039973653</v>
       </c>
-      <c r="O128" s="168">
+      <c r="O128" s="108">
         <v>-25.430708667884439</v>
       </c>
-      <c r="P128" s="168">
+      <c r="P128" s="108">
         <v>-29.012722955393865</v>
       </c>
-      <c r="Q128" s="168">
+      <c r="Q128" s="108">
         <v>-30.711815260688951</v>
       </c>
     </row>
@@ -42751,16 +42722,16 @@
       <c r="M129" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N129" s="168">
+      <c r="N129" s="108">
         <v>2921.9246347006133</v>
       </c>
-      <c r="O129" s="168">
+      <c r="O129" s="108">
         <v>3037.8229476595893</v>
       </c>
-      <c r="P129" s="168">
+      <c r="P129" s="108">
         <v>3063.0520791261606</v>
       </c>
-      <c r="Q129" s="168">
+      <c r="Q129" s="108">
         <v>3071.349945173808</v>
       </c>
     </row>
@@ -42787,16 +42758,16 @@
       <c r="M130" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="N130" s="168">
+      <c r="N130" s="108">
         <v>194.98950459871116</v>
       </c>
-      <c r="O130" s="168">
+      <c r="O130" s="108">
         <v>106.44111613147737</v>
       </c>
-      <c r="P130" s="168">
+      <c r="P130" s="108">
         <v>93.095966030316205</v>
       </c>
-      <c r="Q130" s="168">
+      <c r="Q130" s="108">
         <v>88.683291311747411</v>
       </c>
     </row>
@@ -42820,16 +42791,16 @@
       <c r="L131" s="112" t="s">
         <v>337</v>
       </c>
-      <c r="N131" s="177">
+      <c r="N131" s="153">
         <v>4.6017582296384259E-4</v>
       </c>
-      <c r="O131" s="177">
+      <c r="O131" s="153">
         <v>7.5546787921607918E-4</v>
       </c>
-      <c r="P131" s="177">
+      <c r="P131" s="153">
         <v>8.8171451428223618E-4</v>
       </c>
-      <c r="Q131" s="177">
+      <c r="Q131" s="153">
         <v>9.5553710766224805E-4</v>
       </c>
       <c r="R131" t="s">
@@ -42856,16 +42827,16 @@
       <c r="L132" s="112" t="s">
         <v>338</v>
       </c>
-      <c r="N132" s="177">
+      <c r="N132" s="153">
         <v>0.51266521484210426</v>
       </c>
-      <c r="O132" s="177">
+      <c r="O132" s="153">
         <v>0.4914704113240943</v>
       </c>
-      <c r="P132" s="177">
+      <c r="P132" s="153">
         <v>0.499963695250836</v>
       </c>
-      <c r="Q132" s="177">
+      <c r="Q132" s="153">
         <v>0.5092089511151171</v>
       </c>
       <c r="R132" t="s">
@@ -42892,16 +42863,16 @@
       <c r="L133" s="112" t="s">
         <v>339</v>
       </c>
-      <c r="N133" s="177">
+      <c r="N133" s="153">
         <v>41.803279952114735</v>
       </c>
-      <c r="O133" s="177">
+      <c r="O133" s="153">
         <v>23.679754829388798</v>
       </c>
-      <c r="P133" s="177">
+      <c r="P133" s="153">
         <v>19.225837394967471</v>
       </c>
-      <c r="Q133" s="177">
+      <c r="Q133" s="153">
         <v>17.544443027570992</v>
       </c>
       <c r="R133" t="s">
@@ -42909,22 +42880,22 @@
       </c>
     </row>
     <row r="134" spans="3:18">
-      <c r="N134" s="172"/>
-      <c r="O134" s="172"/>
-      <c r="P134" s="172"/>
-      <c r="Q134" s="172"/>
+      <c r="N134" s="112"/>
+      <c r="O134" s="112"/>
+      <c r="P134" s="112"/>
+      <c r="Q134" s="112"/>
     </row>
     <row r="135" spans="3:18">
-      <c r="N135" s="169">
+      <c r="N135" s="109">
         <v>1.3851703865814915</v>
       </c>
-      <c r="O135" s="169">
+      <c r="O135" s="109">
         <v>3.3665035071317746</v>
       </c>
-      <c r="P135" s="169">
+      <c r="P135" s="109">
         <v>4.9326761741143894</v>
       </c>
-      <c r="Q135" s="169">
+      <c r="Q135" s="109">
         <v>6.1227031146042687</v>
       </c>
     </row>
@@ -43319,20 +43290,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -43355,6 +43326,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -43369,12 +43348,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Nut object to bolts module and added a nut parameter to PolynomialLFlangeSegment
</commit_message>
<xml_diff>
--- a/validations/flangesegments.PolynomialLFlangeSegment/BnB_ReferenceFlange-Results-ShapeFactor-1.2.xlsx
+++ b/validations/flangesegments.PolynomialLFlangeSegment/BnB_ReferenceFlange-Results-ShapeFactor-1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelloB\mdb\!Progetti\!KCI\!SP2200052 - Bolt &amp; Beautiful\!pyflange-package\validations\flangesegments.PolynomialLFlangeSegment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D73949C-CD35-4919-A71D-BDE921882F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D7D40B-E955-42CC-A94A-BC71A13211AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="15" windowWidth="29040" windowHeight="17520" activeTab="3" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
+    <workbookView xWindow="-28920" yWindow="-9165" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Gap30deg" sheetId="2" r:id="rId1"/>
@@ -5501,6 +5501,24 @@
     <xf numFmtId="171" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -5519,26 +5537,8 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -19730,7 +19730,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="45720" tIns="36576" rIns="45720" bIns="36576" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -20144,32 +20144,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="162"/>
-      <c r="C3" s="162"/>
-      <c r="D3" s="162"/>
-      <c r="E3" s="162"/>
-      <c r="F3" s="162"/>
-      <c r="G3" s="162"/>
-      <c r="H3" s="162"/>
-      <c r="I3" s="162"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="162"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+      <c r="I3" s="159"/>
+      <c r="J3" s="159"/>
+      <c r="K3" s="159"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="160" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="160"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -20185,12 +20185,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="155"/>
-      <c r="C5" s="156"/>
-      <c r="D5" s="156"/>
-      <c r="E5" s="156"/>
-      <c r="F5" s="156"/>
-      <c r="G5" s="157"/>
+      <c r="B5" s="161"/>
+      <c r="C5" s="162"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162"/>
+      <c r="G5" s="163"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -20198,12 +20198,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="155"/>
-      <c r="C6" s="156"/>
-      <c r="D6" s="156"/>
-      <c r="E6" s="156"/>
-      <c r="F6" s="156"/>
-      <c r="G6" s="157"/>
+      <c r="B6" s="161"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="163"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -20211,12 +20211,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="155"/>
-      <c r="C7" s="156"/>
-      <c r="D7" s="156"/>
-      <c r="E7" s="156"/>
-      <c r="F7" s="156"/>
-      <c r="G7" s="157"/>
+      <c r="B7" s="161"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="162"/>
+      <c r="E7" s="162"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="163"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -20224,12 +20224,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="155"/>
-      <c r="C8" s="156"/>
-      <c r="D8" s="156"/>
-      <c r="E8" s="156"/>
-      <c r="F8" s="156"/>
-      <c r="G8" s="157"/>
+      <c r="B8" s="161"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162"/>
+      <c r="G8" s="163"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -20237,12 +20237,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="155"/>
-      <c r="C9" s="156"/>
-      <c r="D9" s="156"/>
-      <c r="E9" s="156"/>
-      <c r="F9" s="156"/>
-      <c r="G9" s="157"/>
+      <c r="B9" s="161"/>
+      <c r="C9" s="162"/>
+      <c r="D9" s="162"/>
+      <c r="E9" s="162"/>
+      <c r="F9" s="162"/>
+      <c r="G9" s="163"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -20290,112 +20290,112 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="158" t="s">
+      <c r="B13" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="158"/>
-      <c r="D13" s="160" t="s">
+      <c r="C13" s="164"/>
+      <c r="D13" s="166" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="160"/>
-      <c r="F13" s="160"/>
-      <c r="G13" s="160"/>
-      <c r="H13" s="160"/>
-      <c r="I13" s="160"/>
-      <c r="J13" s="160"/>
-      <c r="K13" s="160"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="166"/>
+      <c r="G13" s="166"/>
+      <c r="H13" s="166"/>
+      <c r="I13" s="166"/>
+      <c r="J13" s="166"/>
+      <c r="K13" s="166"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="158" t="s">
+      <c r="B14" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="158"/>
-      <c r="D14" s="160" t="s">
+      <c r="C14" s="164"/>
+      <c r="D14" s="166" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="160"/>
-      <c r="F14" s="160"/>
-      <c r="G14" s="160"/>
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="160"/>
-      <c r="K14" s="160"/>
+      <c r="E14" s="166"/>
+      <c r="F14" s="166"/>
+      <c r="G14" s="166"/>
+      <c r="H14" s="166"/>
+      <c r="I14" s="166"/>
+      <c r="J14" s="166"/>
+      <c r="K14" s="166"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="158" t="s">
+      <c r="B15" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="158"/>
-      <c r="D15" s="160" t="s">
+      <c r="C15" s="164"/>
+      <c r="D15" s="166" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="160"/>
-      <c r="F15" s="160"/>
-      <c r="G15" s="160"/>
-      <c r="H15" s="160"/>
-      <c r="I15" s="160"/>
-      <c r="J15" s="160"/>
-      <c r="K15" s="160"/>
+      <c r="E15" s="166"/>
+      <c r="F15" s="166"/>
+      <c r="G15" s="166"/>
+      <c r="H15" s="166"/>
+      <c r="I15" s="166"/>
+      <c r="J15" s="166"/>
+      <c r="K15" s="166"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="158" t="s">
+      <c r="B16" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="158"/>
-      <c r="D16" s="160" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="166" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 30° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="160"/>
-      <c r="F16" s="160"/>
-      <c r="G16" s="160"/>
-      <c r="H16" s="160"/>
-      <c r="I16" s="160"/>
-      <c r="J16" s="160"/>
-      <c r="K16" s="160"/>
+      <c r="E16" s="166"/>
+      <c r="F16" s="166"/>
+      <c r="G16" s="166"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="166"/>
+      <c r="J16" s="166"/>
+      <c r="K16" s="166"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="158" t="s">
+      <c r="B17" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="158"/>
-      <c r="D17" s="164">
+      <c r="C17" s="164"/>
+      <c r="D17" s="167">
         <v>0.1</v>
       </c>
-      <c r="E17" s="160"/>
-      <c r="F17" s="160"/>
-      <c r="G17" s="160"/>
-      <c r="H17" s="160"/>
-      <c r="I17" s="160"/>
-      <c r="J17" s="160"/>
-      <c r="K17" s="160"/>
+      <c r="E17" s="166"/>
+      <c r="F17" s="166"/>
+      <c r="G17" s="166"/>
+      <c r="H17" s="166"/>
+      <c r="I17" s="166"/>
+      <c r="J17" s="166"/>
+      <c r="K17" s="166"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="158" t="s">
+      <c r="B18" s="164" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="158"/>
-      <c r="D18" s="159">
+      <c r="C18" s="164"/>
+      <c r="D18" s="165">
         <v>45432</v>
       </c>
-      <c r="E18" s="159"/>
-      <c r="F18" s="159"/>
-      <c r="G18" s="159"/>
-      <c r="H18" s="159"/>
-      <c r="I18" s="159"/>
-      <c r="J18" s="159"/>
-      <c r="K18" s="159"/>
+      <c r="E18" s="165"/>
+      <c r="F18" s="165"/>
+      <c r="G18" s="165"/>
+      <c r="H18" s="165"/>
+      <c r="I18" s="165"/>
+      <c r="J18" s="165"/>
+      <c r="K18" s="165"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -20583,16 +20583,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="165"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
-      <c r="H28" s="166"/>
-      <c r="I28" s="166"/>
-      <c r="J28" s="166"/>
-      <c r="K28" s="167"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
+      <c r="K28" s="157"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -24555,6 +24555,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:K15"/>
+    <mergeCell ref="B13:C13"/>
     <mergeCell ref="B28:K28"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="B4:G4"/>
@@ -24571,10 +24575,6 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:K15"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="27" priority="5" stopIfTrue="1" operator="between">
@@ -24660,32 +24660,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="162"/>
-      <c r="C3" s="162"/>
-      <c r="D3" s="162"/>
-      <c r="E3" s="162"/>
-      <c r="F3" s="162"/>
-      <c r="G3" s="162"/>
-      <c r="H3" s="162"/>
-      <c r="I3" s="162"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="162"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+      <c r="I3" s="159"/>
+      <c r="J3" s="159"/>
+      <c r="K3" s="159"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="160" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="160"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -24701,12 +24701,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="155"/>
-      <c r="C5" s="156"/>
-      <c r="D5" s="156"/>
-      <c r="E5" s="156"/>
-      <c r="F5" s="156"/>
-      <c r="G5" s="157"/>
+      <c r="B5" s="161"/>
+      <c r="C5" s="162"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162"/>
+      <c r="G5" s="163"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -24714,12 +24714,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="155"/>
-      <c r="C6" s="156"/>
-      <c r="D6" s="156"/>
-      <c r="E6" s="156"/>
-      <c r="F6" s="156"/>
-      <c r="G6" s="157"/>
+      <c r="B6" s="161"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="163"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -24727,12 +24727,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="155"/>
-      <c r="C7" s="156"/>
-      <c r="D7" s="156"/>
-      <c r="E7" s="156"/>
-      <c r="F7" s="156"/>
-      <c r="G7" s="157"/>
+      <c r="B7" s="161"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="162"/>
+      <c r="E7" s="162"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="163"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -24740,12 +24740,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="155"/>
-      <c r="C8" s="156"/>
-      <c r="D8" s="156"/>
-      <c r="E8" s="156"/>
-      <c r="F8" s="156"/>
-      <c r="G8" s="157"/>
+      <c r="B8" s="161"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162"/>
+      <c r="G8" s="163"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -24753,12 +24753,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="155"/>
-      <c r="C9" s="156"/>
-      <c r="D9" s="156"/>
-      <c r="E9" s="156"/>
-      <c r="F9" s="156"/>
-      <c r="G9" s="157"/>
+      <c r="B9" s="161"/>
+      <c r="C9" s="162"/>
+      <c r="D9" s="162"/>
+      <c r="E9" s="162"/>
+      <c r="F9" s="162"/>
+      <c r="G9" s="163"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -24806,117 +24806,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="158" t="s">
+      <c r="B13" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="158"/>
-      <c r="D13" s="160" t="str">
+      <c r="C13" s="164"/>
+      <c r="D13" s="166" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="160"/>
-      <c r="F13" s="160"/>
-      <c r="G13" s="160"/>
-      <c r="H13" s="160"/>
-      <c r="I13" s="160"/>
-      <c r="J13" s="160"/>
-      <c r="K13" s="160"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="166"/>
+      <c r="G13" s="166"/>
+      <c r="H13" s="166"/>
+      <c r="I13" s="166"/>
+      <c r="J13" s="166"/>
+      <c r="K13" s="166"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="158" t="s">
+      <c r="B14" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="158"/>
-      <c r="D14" s="160" t="str">
+      <c r="C14" s="164"/>
+      <c r="D14" s="166" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="160"/>
-      <c r="F14" s="160"/>
-      <c r="G14" s="160"/>
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="160"/>
-      <c r="K14" s="160"/>
+      <c r="E14" s="166"/>
+      <c r="F14" s="166"/>
+      <c r="G14" s="166"/>
+      <c r="H14" s="166"/>
+      <c r="I14" s="166"/>
+      <c r="J14" s="166"/>
+      <c r="K14" s="166"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="158" t="s">
+      <c r="B15" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="158"/>
-      <c r="D15" s="160" t="str">
+      <c r="C15" s="164"/>
+      <c r="D15" s="166" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="160"/>
-      <c r="F15" s="160"/>
-      <c r="G15" s="160"/>
-      <c r="H15" s="160"/>
-      <c r="I15" s="160"/>
-      <c r="J15" s="160"/>
-      <c r="K15" s="160"/>
+      <c r="E15" s="166"/>
+      <c r="F15" s="166"/>
+      <c r="G15" s="166"/>
+      <c r="H15" s="166"/>
+      <c r="I15" s="166"/>
+      <c r="J15" s="166"/>
+      <c r="K15" s="166"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="158" t="s">
+      <c r="B16" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="158"/>
-      <c r="D16" s="160" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="166" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 60° gap size ans shape factor 1.2</v>
       </c>
-      <c r="E16" s="160"/>
-      <c r="F16" s="160"/>
-      <c r="G16" s="160"/>
-      <c r="H16" s="160"/>
-      <c r="I16" s="160"/>
-      <c r="J16" s="160"/>
-      <c r="K16" s="160"/>
+      <c r="E16" s="166"/>
+      <c r="F16" s="166"/>
+      <c r="G16" s="166"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="166"/>
+      <c r="J16" s="166"/>
+      <c r="K16" s="166"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="158" t="s">
+      <c r="B17" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="158"/>
-      <c r="D17" s="160">
+      <c r="C17" s="164"/>
+      <c r="D17" s="166">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="160"/>
-      <c r="F17" s="160"/>
-      <c r="G17" s="160"/>
-      <c r="H17" s="160"/>
-      <c r="I17" s="160"/>
-      <c r="J17" s="160"/>
-      <c r="K17" s="160"/>
+      <c r="E17" s="166"/>
+      <c r="F17" s="166"/>
+      <c r="G17" s="166"/>
+      <c r="H17" s="166"/>
+      <c r="I17" s="166"/>
+      <c r="J17" s="166"/>
+      <c r="K17" s="166"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="158" t="s">
+      <c r="B18" s="164" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="158"/>
-      <c r="D18" s="159">
+      <c r="C18" s="164"/>
+      <c r="D18" s="165">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="159"/>
-      <c r="F18" s="159"/>
-      <c r="G18" s="159"/>
-      <c r="H18" s="159"/>
-      <c r="I18" s="159"/>
-      <c r="J18" s="159"/>
-      <c r="K18" s="159"/>
+      <c r="E18" s="165"/>
+      <c r="F18" s="165"/>
+      <c r="G18" s="165"/>
+      <c r="H18" s="165"/>
+      <c r="I18" s="165"/>
+      <c r="J18" s="165"/>
+      <c r="K18" s="165"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -25104,16 +25104,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="165"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
-      <c r="H28" s="166"/>
-      <c r="I28" s="166"/>
-      <c r="J28" s="166"/>
-      <c r="K28" s="167"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
+      <c r="K28" s="157"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -29039,13 +29039,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -29059,6 +29052,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="24" priority="3" stopIfTrue="1" operator="between">
@@ -29144,32 +29144,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="162"/>
-      <c r="C3" s="162"/>
-      <c r="D3" s="162"/>
-      <c r="E3" s="162"/>
-      <c r="F3" s="162"/>
-      <c r="G3" s="162"/>
-      <c r="H3" s="162"/>
-      <c r="I3" s="162"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="162"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+      <c r="I3" s="159"/>
+      <c r="J3" s="159"/>
+      <c r="K3" s="159"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="160" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="160"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -29185,12 +29185,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="155"/>
-      <c r="C5" s="156"/>
-      <c r="D5" s="156"/>
-      <c r="E5" s="156"/>
-      <c r="F5" s="156"/>
-      <c r="G5" s="157"/>
+      <c r="B5" s="161"/>
+      <c r="C5" s="162"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162"/>
+      <c r="G5" s="163"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -29198,12 +29198,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="155"/>
-      <c r="C6" s="156"/>
-      <c r="D6" s="156"/>
-      <c r="E6" s="156"/>
-      <c r="F6" s="156"/>
-      <c r="G6" s="157"/>
+      <c r="B6" s="161"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="163"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -29211,12 +29211,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="155"/>
-      <c r="C7" s="156"/>
-      <c r="D7" s="156"/>
-      <c r="E7" s="156"/>
-      <c r="F7" s="156"/>
-      <c r="G7" s="157"/>
+      <c r="B7" s="161"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="162"/>
+      <c r="E7" s="162"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="163"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -29224,12 +29224,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="155"/>
-      <c r="C8" s="156"/>
-      <c r="D8" s="156"/>
-      <c r="E8" s="156"/>
-      <c r="F8" s="156"/>
-      <c r="G8" s="157"/>
+      <c r="B8" s="161"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162"/>
+      <c r="G8" s="163"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -29237,12 +29237,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="155"/>
-      <c r="C9" s="156"/>
-      <c r="D9" s="156"/>
-      <c r="E9" s="156"/>
-      <c r="F9" s="156"/>
-      <c r="G9" s="157"/>
+      <c r="B9" s="161"/>
+      <c r="C9" s="162"/>
+      <c r="D9" s="162"/>
+      <c r="E9" s="162"/>
+      <c r="F9" s="162"/>
+      <c r="G9" s="163"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -29290,117 +29290,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="158" t="s">
+      <c r="B13" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="158"/>
-      <c r="D13" s="160" t="str">
+      <c r="C13" s="164"/>
+      <c r="D13" s="166" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="160"/>
-      <c r="F13" s="160"/>
-      <c r="G13" s="160"/>
-      <c r="H13" s="160"/>
-      <c r="I13" s="160"/>
-      <c r="J13" s="160"/>
-      <c r="K13" s="160"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="166"/>
+      <c r="G13" s="166"/>
+      <c r="H13" s="166"/>
+      <c r="I13" s="166"/>
+      <c r="J13" s="166"/>
+      <c r="K13" s="166"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="158" t="s">
+      <c r="B14" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="158"/>
-      <c r="D14" s="160" t="str">
+      <c r="C14" s="164"/>
+      <c r="D14" s="166" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="160"/>
-      <c r="F14" s="160"/>
-      <c r="G14" s="160"/>
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="160"/>
-      <c r="K14" s="160"/>
+      <c r="E14" s="166"/>
+      <c r="F14" s="166"/>
+      <c r="G14" s="166"/>
+      <c r="H14" s="166"/>
+      <c r="I14" s="166"/>
+      <c r="J14" s="166"/>
+      <c r="K14" s="166"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="158" t="s">
+      <c r="B15" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="158"/>
-      <c r="D15" s="160" t="str">
+      <c r="C15" s="164"/>
+      <c r="D15" s="166" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="160"/>
-      <c r="F15" s="160"/>
-      <c r="G15" s="160"/>
-      <c r="H15" s="160"/>
-      <c r="I15" s="160"/>
-      <c r="J15" s="160"/>
-      <c r="K15" s="160"/>
+      <c r="E15" s="166"/>
+      <c r="F15" s="166"/>
+      <c r="G15" s="166"/>
+      <c r="H15" s="166"/>
+      <c r="I15" s="166"/>
+      <c r="J15" s="166"/>
+      <c r="K15" s="166"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="158" t="s">
+      <c r="B16" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="158"/>
-      <c r="D16" s="160" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="166" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 90° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="160"/>
-      <c r="F16" s="160"/>
-      <c r="G16" s="160"/>
-      <c r="H16" s="160"/>
-      <c r="I16" s="160"/>
-      <c r="J16" s="160"/>
-      <c r="K16" s="160"/>
+      <c r="E16" s="166"/>
+      <c r="F16" s="166"/>
+      <c r="G16" s="166"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="166"/>
+      <c r="J16" s="166"/>
+      <c r="K16" s="166"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="158" t="s">
+      <c r="B17" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="158"/>
-      <c r="D17" s="160">
+      <c r="C17" s="164"/>
+      <c r="D17" s="166">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="160"/>
-      <c r="F17" s="160"/>
-      <c r="G17" s="160"/>
-      <c r="H17" s="160"/>
-      <c r="I17" s="160"/>
-      <c r="J17" s="160"/>
-      <c r="K17" s="160"/>
+      <c r="E17" s="166"/>
+      <c r="F17" s="166"/>
+      <c r="G17" s="166"/>
+      <c r="H17" s="166"/>
+      <c r="I17" s="166"/>
+      <c r="J17" s="166"/>
+      <c r="K17" s="166"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="158" t="s">
+      <c r="B18" s="164" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="158"/>
-      <c r="D18" s="159">
+      <c r="C18" s="164"/>
+      <c r="D18" s="165">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="159"/>
-      <c r="F18" s="159"/>
-      <c r="G18" s="159"/>
-      <c r="H18" s="159"/>
-      <c r="I18" s="159"/>
-      <c r="J18" s="159"/>
-      <c r="K18" s="159"/>
+      <c r="E18" s="165"/>
+      <c r="F18" s="165"/>
+      <c r="G18" s="165"/>
+      <c r="H18" s="165"/>
+      <c r="I18" s="165"/>
+      <c r="J18" s="165"/>
+      <c r="K18" s="165"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -29588,16 +29588,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="165"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
-      <c r="H28" s="166"/>
-      <c r="I28" s="166"/>
-      <c r="J28" s="166"/>
-      <c r="K28" s="167"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
+      <c r="K28" s="157"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -33523,13 +33523,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -33543,6 +33536,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="between">
@@ -33581,7 +33581,7 @@
   </sheetPr>
   <dimension ref="A1:DJ180"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="O117" sqref="O117"/>
     </sheetView>
@@ -33628,32 +33628,32 @@
       <c r="K2" s="48"/>
     </row>
     <row r="3" spans="1:15" ht="54.75" hidden="1" customHeight="1" outlineLevel="1">
-      <c r="A3" s="161" t="s">
+      <c r="A3" s="158" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="162"/>
-      <c r="C3" s="162"/>
-      <c r="D3" s="162"/>
-      <c r="E3" s="162"/>
-      <c r="F3" s="162"/>
-      <c r="G3" s="162"/>
-      <c r="H3" s="162"/>
-      <c r="I3" s="162"/>
-      <c r="J3" s="162"/>
-      <c r="K3" s="162"/>
+      <c r="B3" s="159"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+      <c r="I3" s="159"/>
+      <c r="J3" s="159"/>
+      <c r="K3" s="159"/>
     </row>
     <row r="4" spans="1:15" s="46" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="163" t="s">
+      <c r="B4" s="160" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="163"/>
-      <c r="D4" s="163"/>
-      <c r="E4" s="163"/>
-      <c r="F4" s="163"/>
-      <c r="G4" s="163"/>
+      <c r="C4" s="160"/>
+      <c r="D4" s="160"/>
+      <c r="E4" s="160"/>
+      <c r="F4" s="160"/>
+      <c r="G4" s="160"/>
       <c r="H4" s="47" t="s">
         <v>13</v>
       </c>
@@ -33669,12 +33669,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="155"/>
-      <c r="C5" s="156"/>
-      <c r="D5" s="156"/>
-      <c r="E5" s="156"/>
-      <c r="F5" s="156"/>
-      <c r="G5" s="157"/>
+      <c r="B5" s="161"/>
+      <c r="C5" s="162"/>
+      <c r="D5" s="162"/>
+      <c r="E5" s="162"/>
+      <c r="F5" s="162"/>
+      <c r="G5" s="163"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -33682,12 +33682,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="155"/>
-      <c r="C6" s="156"/>
-      <c r="D6" s="156"/>
-      <c r="E6" s="156"/>
-      <c r="F6" s="156"/>
-      <c r="G6" s="157"/>
+      <c r="B6" s="161"/>
+      <c r="C6" s="162"/>
+      <c r="D6" s="162"/>
+      <c r="E6" s="162"/>
+      <c r="F6" s="162"/>
+      <c r="G6" s="163"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -33695,12 +33695,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="155"/>
-      <c r="C7" s="156"/>
-      <c r="D7" s="156"/>
-      <c r="E7" s="156"/>
-      <c r="F7" s="156"/>
-      <c r="G7" s="157"/>
+      <c r="B7" s="161"/>
+      <c r="C7" s="162"/>
+      <c r="D7" s="162"/>
+      <c r="E7" s="162"/>
+      <c r="F7" s="162"/>
+      <c r="G7" s="163"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -33708,12 +33708,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="155"/>
-      <c r="C8" s="156"/>
-      <c r="D8" s="156"/>
-      <c r="E8" s="156"/>
-      <c r="F8" s="156"/>
-      <c r="G8" s="157"/>
+      <c r="B8" s="161"/>
+      <c r="C8" s="162"/>
+      <c r="D8" s="162"/>
+      <c r="E8" s="162"/>
+      <c r="F8" s="162"/>
+      <c r="G8" s="163"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -33721,12 +33721,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="155"/>
-      <c r="C9" s="156"/>
-      <c r="D9" s="156"/>
-      <c r="E9" s="156"/>
-      <c r="F9" s="156"/>
-      <c r="G9" s="157"/>
+      <c r="B9" s="161"/>
+      <c r="C9" s="162"/>
+      <c r="D9" s="162"/>
+      <c r="E9" s="162"/>
+      <c r="F9" s="162"/>
+      <c r="G9" s="163"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -33774,117 +33774,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="158" t="s">
+      <c r="B13" s="164" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="158"/>
-      <c r="D13" s="160" t="str">
+      <c r="C13" s="164"/>
+      <c r="D13" s="166" t="str">
         <f>Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="160"/>
-      <c r="F13" s="160"/>
-      <c r="G13" s="160"/>
-      <c r="H13" s="160"/>
-      <c r="I13" s="160"/>
-      <c r="J13" s="160"/>
-      <c r="K13" s="160"/>
+      <c r="E13" s="166"/>
+      <c r="F13" s="166"/>
+      <c r="G13" s="166"/>
+      <c r="H13" s="166"/>
+      <c r="I13" s="166"/>
+      <c r="J13" s="166"/>
+      <c r="K13" s="166"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="158" t="s">
+      <c r="B14" s="164" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="158"/>
-      <c r="D14" s="160" t="str">
+      <c r="C14" s="164"/>
+      <c r="D14" s="166" t="str">
         <f>Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="160"/>
-      <c r="F14" s="160"/>
-      <c r="G14" s="160"/>
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="160"/>
-      <c r="K14" s="160"/>
+      <c r="E14" s="166"/>
+      <c r="F14" s="166"/>
+      <c r="G14" s="166"/>
+      <c r="H14" s="166"/>
+      <c r="I14" s="166"/>
+      <c r="J14" s="166"/>
+      <c r="K14" s="166"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="158" t="s">
+      <c r="B15" s="164" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="158"/>
-      <c r="D15" s="160" t="str">
+      <c r="C15" s="164"/>
+      <c r="D15" s="166" t="str">
         <f>Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="160"/>
-      <c r="F15" s="160"/>
-      <c r="G15" s="160"/>
-      <c r="H15" s="160"/>
-      <c r="I15" s="160"/>
-      <c r="J15" s="160"/>
-      <c r="K15" s="160"/>
+      <c r="E15" s="166"/>
+      <c r="F15" s="166"/>
+      <c r="G15" s="166"/>
+      <c r="H15" s="166"/>
+      <c r="I15" s="166"/>
+      <c r="J15" s="166"/>
+      <c r="K15" s="166"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="158" t="s">
+      <c r="B16" s="164" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="158"/>
-      <c r="D16" s="160" t="str">
+      <c r="C16" s="164"/>
+      <c r="D16" s="166" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 120° gap size and shape factor 1.2</v>
       </c>
-      <c r="E16" s="160"/>
-      <c r="F16" s="160"/>
-      <c r="G16" s="160"/>
-      <c r="H16" s="160"/>
-      <c r="I16" s="160"/>
-      <c r="J16" s="160"/>
-      <c r="K16" s="160"/>
+      <c r="E16" s="166"/>
+      <c r="F16" s="166"/>
+      <c r="G16" s="166"/>
+      <c r="H16" s="166"/>
+      <c r="I16" s="166"/>
+      <c r="J16" s="166"/>
+      <c r="K16" s="166"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="158" t="s">
+      <c r="B17" s="164" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="158"/>
-      <c r="D17" s="160">
+      <c r="C17" s="164"/>
+      <c r="D17" s="166">
         <f>Gap30deg!D17</f>
         <v>0.1</v>
       </c>
-      <c r="E17" s="160"/>
-      <c r="F17" s="160"/>
-      <c r="G17" s="160"/>
-      <c r="H17" s="160"/>
-      <c r="I17" s="160"/>
-      <c r="J17" s="160"/>
-      <c r="K17" s="160"/>
+      <c r="E17" s="166"/>
+      <c r="F17" s="166"/>
+      <c r="G17" s="166"/>
+      <c r="H17" s="166"/>
+      <c r="I17" s="166"/>
+      <c r="J17" s="166"/>
+      <c r="K17" s="166"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="158" t="s">
+      <c r="B18" s="164" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="158"/>
-      <c r="D18" s="159">
+      <c r="C18" s="164"/>
+      <c r="D18" s="165">
         <f>Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="159"/>
-      <c r="F18" s="159"/>
-      <c r="G18" s="159"/>
-      <c r="H18" s="159"/>
-      <c r="I18" s="159"/>
-      <c r="J18" s="159"/>
-      <c r="K18" s="159"/>
+      <c r="E18" s="165"/>
+      <c r="F18" s="165"/>
+      <c r="G18" s="165"/>
+      <c r="H18" s="165"/>
+      <c r="I18" s="165"/>
+      <c r="J18" s="165"/>
+      <c r="K18" s="165"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -34072,16 +34072,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="165"/>
-      <c r="C28" s="166"/>
-      <c r="D28" s="166"/>
-      <c r="E28" s="166"/>
-      <c r="F28" s="166"/>
-      <c r="G28" s="166"/>
-      <c r="H28" s="166"/>
-      <c r="I28" s="166"/>
-      <c r="J28" s="166"/>
-      <c r="K28" s="167"/>
+      <c r="B28" s="155"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
+      <c r="K28" s="157"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -38007,13 +38007,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -38027,6 +38020,13 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
     <cfRule type="cellIs" dxfId="18" priority="3" stopIfTrue="1" operator="between">
@@ -38063,12 +38063,12 @@
   <sheetPr codeName="Tabelle12"/>
   <dimension ref="B2:R135"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="21" topLeftCell="B107" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="21" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
       <selection pane="topRight" activeCell="B6" sqref="B6"/>
       <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
-      <selection pane="bottomRight" activeCell="N25" sqref="N25"/>
+      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -42996,7 +42996,7 @@
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G21" xr:uid="{A97D2F7B-FDA4-407E-92F3-17F2D0816A54}">
       <formula1>$N$48:$Q$48</formula1>
     </dataValidation>
@@ -43037,6 +43037,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004E5A98ECA1EC044BB77E0D7F6ADEF7BC" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="5e88349ac6f5efd4674595e2a92e1fa9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2278e7f3-5df8-4100-b836-5320443b7544" xmlns:ns4="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bde21b231255bb48ab8a6ec7dd561648" ns3:_="" ns4:_="">
     <xsd:import namespace="2278e7f3-5df8-4100-b836-5320443b7544"/>
@@ -43289,24 +43306,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
+    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A7863D2-B6F1-4C67-B9E9-1F3A9276C4FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -43323,29 +43348,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
-    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>